<commit_message>
V1.0.4 Additional Cases of Profile Editor & Change Password | Updated Manual TestCases
</commit_message>
<xml_diff>
--- a/TestCases_of _Idx-Auto-Tester.xlsx
+++ b/TestCases_of _Idx-Auto-Tester.xlsx
@@ -3,15 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="TC_Registration" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="TC_BasicFeatures" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
+  <extLst>
+    <ext uri="GoogleSheetsCustomDataVersion1">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mhxYweP5EbOGbpw72DIihzgG+xLtw=="/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
   <si>
     <t>Test case ID</t>
   </si>
@@ -309,10 +314,50 @@
     <t>User should receive error message of 'Your current password is invalid, please use the correct password.' and should unable to change password.</t>
   </si>
   <si>
+    <t>TC_18</t>
+  </si>
+  <si>
+    <t>Verify that user is getting proper error message on blank fields submission</t>
+  </si>
+  <si>
+    <t>1. Create user by account api with sample payload using loginradius-sdk 
+2. Navigate to Site URL
+3. Navigate to Login Page
+4. Enter Email Id and Password which used in sample payload
+5. Click on Login button 
+6. Check that navigated to profile page
+7. Navigate to Account Menu &gt; Change Password
+8. Leave Current Password and New Password, Confirm Password fields blank
+9. Click on Submit button</t>
+  </si>
+  <si>
+    <t>User should receive error message for all required blank fields.</t>
+  </si>
+  <si>
+    <t>TC_19</t>
+  </si>
+  <si>
+    <t>Verify that user is unable to change password when new and confirm password mismatch</t>
+  </si>
+  <si>
+    <t>1. Create user by account api with sample payload using loginradius-sdk 
+2. Navigate to Site URL
+3. Navigate to Login Page
+4. Enter Email Id and Password which used in sample payload
+5. Click on Login button 
+6. Check that navigated to profile page
+7. Navigate to Account Menu &gt; Change Password
+8. Enter valid Current Password and mismatch values in New Password, Confirm Password
+9. Click on Submit button</t>
+  </si>
+  <si>
+    <t>User should receive error message of 'The Confirm Password field does not match the Password field.'</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Cases of Profile Editor Feature </t>
   </si>
   <si>
-    <t>TC_18</t>
+    <t>TC_20</t>
   </si>
   <si>
     <t>Verify that user is able to update profile after logged-in</t>
@@ -333,10 +378,30 @@
     <t>User should able to update profile successfully with new data.</t>
   </si>
   <si>
+    <t>TC_21</t>
+  </si>
+  <si>
+    <t>Verify that user is able to update profile with blank last name field</t>
+  </si>
+  <si>
+    <t>1. Create user by account api with sample payload using loginradius-sdk 
+2. Navigate to Site URL
+3. Navigate to Login Page
+4. Enter Email Id and Password which used in sample payload
+5. Click on Login button 
+6. Check that navigated to profile page
+7. Navigate to Account Menu &gt; Edit Profile
+8. Clear already entered data of Last Name
+9. Click on Submit button</t>
+  </si>
+  <si>
+    <t>User should able to update profile successfully with blank Last Name field.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test Cases of Forgot Password Feature </t>
   </si>
   <si>
-    <t>TC_19</t>
+    <t>TC_22</t>
   </si>
   <si>
     <t>Verify that user is able to reset password by using forgot password option</t>
@@ -362,7 +427,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -386,8 +451,12 @@
       <sz val="10.0"/>
       <color rgb="FF032F62"/>
     </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,6 +475,12 @@
         <bgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -413,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -438,17 +513,30 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -739,7 +827,7 @@
       <c r="X2" s="4"/>
       <c r="Y2" s="4"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -774,7 +862,7 @@
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
@@ -809,7 +897,7 @@
       <c r="X4" s="4"/>
       <c r="Y4" s="4"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5">
       <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
@@ -844,7 +932,7 @@
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -879,7 +967,7 @@
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -914,7 +1002,7 @@
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8">
       <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
@@ -949,7 +1037,7 @@
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9">
       <c r="A9" s="4" t="s">
         <v>30</v>
       </c>
@@ -984,7 +1072,7 @@
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10">
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
@@ -1044,18 +1132,18 @@
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="8" t="s">
+    <row r="12">
+      <c r="A12" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="6" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="7" t="s">
         <v>42</v>
       </c>
       <c r="F12" s="4"/>
@@ -1079,18 +1167,18 @@
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="8" t="s">
+    <row r="13">
+      <c r="A13" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="6" t="s">
+      <c r="D13" s="4"/>
+      <c r="E13" s="7" t="s">
         <v>46</v>
       </c>
       <c r="F13" s="4"/>
@@ -1114,18 +1202,18 @@
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="8" t="s">
+    <row r="14">
+      <c r="A14" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="6" t="s">
+      <c r="D14" s="4"/>
+      <c r="E14" s="7" t="s">
         <v>46</v>
       </c>
       <c r="F14" s="4"/>
@@ -1149,18 +1237,18 @@
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="9" t="s">
+    <row r="15">
+      <c r="A15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="11" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="7" t="s">
         <v>53</v>
       </c>
       <c r="F15" s="4"/>
@@ -1184,18 +1272,18 @@
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="9" t="s">
+    <row r="16">
+      <c r="A16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="11" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="7" t="s">
         <v>57</v>
       </c>
       <c r="F16" s="4"/>
@@ -1244,18 +1332,18 @@
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="9" t="s">
+    <row r="18">
+      <c r="A18" s="4" t="s">
         <v>59</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="6" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="7" t="s">
         <v>62</v>
       </c>
       <c r="F18" s="4"/>
@@ -1279,18 +1367,18 @@
       <c r="X18" s="4"/>
       <c r="Y18" s="4"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="9" t="s">
+    <row r="19">
+      <c r="A19" s="4" t="s">
         <v>63</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="6" t="s">
+      <c r="D19" s="4"/>
+      <c r="E19" s="7" t="s">
         <v>66</v>
       </c>
       <c r="F19" s="4"/>
@@ -1339,18 +1427,18 @@
       <c r="X20" s="4"/>
       <c r="Y20" s="4"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="9" t="s">
+    <row r="21">
+      <c r="A21" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="6" t="s">
+      <c r="D21" s="4"/>
+      <c r="E21" s="7" t="s">
         <v>71</v>
       </c>
       <c r="F21" s="4"/>
@@ -1374,18 +1462,18 @@
       <c r="X21" s="4"/>
       <c r="Y21" s="4"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="9" t="s">
+    <row r="22">
+      <c r="A22" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="6" t="s">
+      <c r="D22" s="4"/>
+      <c r="E22" s="7" t="s">
         <v>75</v>
       </c>
       <c r="F22" s="4"/>
@@ -1409,69 +1497,81 @@
       <c r="X22" s="4"/>
       <c r="Y22" s="4"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="5" t="s">
+    <row r="23">
+      <c r="A23" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
-      <c r="O23" s="4"/>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
-      <c r="Y23" s="4"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
+      <c r="B23" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
+      <c r="W23" s="13"/>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="13"/>
+      <c r="Z23" s="14"/>
+    </row>
+    <row r="24">
       <c r="A24" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4"/>
-      <c r="P24" s="4"/>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
-      <c r="T24" s="4"/>
-      <c r="U24" s="4"/>
-      <c r="V24" s="4"/>
-      <c r="W24" s="4"/>
-      <c r="X24" s="4"/>
-      <c r="Y24" s="4"/>
+      <c r="B24" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13"/>
+      <c r="W24" s="13"/>
+      <c r="X24" s="13"/>
+      <c r="Y24" s="13"/>
+      <c r="Z24" s="14"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -1494,19 +1594,19 @@
       <c r="X25" s="4"/>
       <c r="Y25" s="4"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="9" t="s">
-        <v>82</v>
+    <row r="26">
+      <c r="A26" s="16" t="s">
+        <v>85</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="D26" s="4"/>
-      <c r="E26" s="6" t="s">
-        <v>85</v>
+      <c r="E26" s="7" t="s">
+        <v>88</v>
       </c>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
@@ -1529,12 +1629,20 @@
       <c r="X26" s="4"/>
       <c r="Y26" s="4"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="4"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="7"/>
+    <row r="27">
+      <c r="A27" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>91</v>
+      </c>
       <c r="D27" s="4"/>
-      <c r="E27" s="7"/>
+      <c r="E27" s="11" t="s">
+        <v>92</v>
+      </c>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
@@ -1557,11 +1665,9 @@
       <c r="Y27" s="4"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="4"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="7"/>
+      <c r="A28" s="5" t="s">
+        <v>93</v>
+      </c>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
@@ -1583,12 +1689,20 @@
       <c r="X28" s="4"/>
       <c r="Y28" s="4"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="4"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
+    <row r="29">
+      <c r="A29" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>96</v>
+      </c>
       <c r="D29" s="4"/>
-      <c r="E29" s="7"/>
+      <c r="E29" s="7" t="s">
+        <v>97</v>
+      </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
@@ -6930,2332 +7044,2407 @@
       <c r="Y226" s="4"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="B227" s="12"/>
+      <c r="A227" s="4"/>
+      <c r="B227" s="6"/>
+      <c r="C227" s="7"/>
+      <c r="D227" s="4"/>
+      <c r="E227" s="7"/>
+      <c r="F227" s="4"/>
+      <c r="G227" s="4"/>
+      <c r="H227" s="4"/>
+      <c r="I227" s="4"/>
+      <c r="J227" s="4"/>
+      <c r="K227" s="4"/>
+      <c r="L227" s="4"/>
+      <c r="M227" s="4"/>
+      <c r="N227" s="4"/>
+      <c r="O227" s="4"/>
+      <c r="P227" s="4"/>
+      <c r="Q227" s="4"/>
+      <c r="R227" s="4"/>
+      <c r="S227" s="4"/>
+      <c r="T227" s="4"/>
+      <c r="U227" s="4"/>
+      <c r="V227" s="4"/>
+      <c r="W227" s="4"/>
+      <c r="X227" s="4"/>
+      <c r="Y227" s="4"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="B228" s="12"/>
+      <c r="A228" s="4"/>
+      <c r="B228" s="6"/>
+      <c r="C228" s="7"/>
+      <c r="D228" s="4"/>
+      <c r="E228" s="7"/>
+      <c r="F228" s="4"/>
+      <c r="G228" s="4"/>
+      <c r="H228" s="4"/>
+      <c r="I228" s="4"/>
+      <c r="J228" s="4"/>
+      <c r="K228" s="4"/>
+      <c r="L228" s="4"/>
+      <c r="M228" s="4"/>
+      <c r="N228" s="4"/>
+      <c r="O228" s="4"/>
+      <c r="P228" s="4"/>
+      <c r="Q228" s="4"/>
+      <c r="R228" s="4"/>
+      <c r="S228" s="4"/>
+      <c r="T228" s="4"/>
+      <c r="U228" s="4"/>
+      <c r="V228" s="4"/>
+      <c r="W228" s="4"/>
+      <c r="X228" s="4"/>
+      <c r="Y228" s="4"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="B229" s="12"/>
+      <c r="A229" s="4"/>
+      <c r="B229" s="6"/>
+      <c r="C229" s="7"/>
+      <c r="D229" s="4"/>
+      <c r="E229" s="7"/>
+      <c r="F229" s="4"/>
+      <c r="G229" s="4"/>
+      <c r="H229" s="4"/>
+      <c r="I229" s="4"/>
+      <c r="J229" s="4"/>
+      <c r="K229" s="4"/>
+      <c r="L229" s="4"/>
+      <c r="M229" s="4"/>
+      <c r="N229" s="4"/>
+      <c r="O229" s="4"/>
+      <c r="P229" s="4"/>
+      <c r="Q229" s="4"/>
+      <c r="R229" s="4"/>
+      <c r="S229" s="4"/>
+      <c r="T229" s="4"/>
+      <c r="U229" s="4"/>
+      <c r="V229" s="4"/>
+      <c r="W229" s="4"/>
+      <c r="X229" s="4"/>
+      <c r="Y229" s="4"/>
     </row>
     <row r="230" ht="15.75" customHeight="1">
-      <c r="B230" s="12"/>
+      <c r="B230" s="17"/>
     </row>
     <row r="231" ht="15.75" customHeight="1">
-      <c r="B231" s="12"/>
+      <c r="B231" s="17"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="B232" s="12"/>
+      <c r="B232" s="17"/>
     </row>
     <row r="233" ht="15.75" customHeight="1">
-      <c r="B233" s="12"/>
+      <c r="B233" s="17"/>
     </row>
     <row r="234" ht="15.75" customHeight="1">
-      <c r="B234" s="12"/>
+      <c r="B234" s="17"/>
     </row>
     <row r="235" ht="15.75" customHeight="1">
-      <c r="B235" s="12"/>
+      <c r="B235" s="17"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="B236" s="12"/>
+      <c r="B236" s="17"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="B237" s="12"/>
+      <c r="B237" s="17"/>
     </row>
     <row r="238" ht="15.75" customHeight="1">
-      <c r="B238" s="12"/>
+      <c r="B238" s="17"/>
     </row>
     <row r="239" ht="15.75" customHeight="1">
-      <c r="B239" s="12"/>
+      <c r="B239" s="17"/>
     </row>
     <row r="240" ht="15.75" customHeight="1">
-      <c r="B240" s="12"/>
+      <c r="B240" s="17"/>
     </row>
     <row r="241" ht="15.75" customHeight="1">
-      <c r="B241" s="12"/>
+      <c r="B241" s="17"/>
     </row>
     <row r="242" ht="15.75" customHeight="1">
-      <c r="B242" s="12"/>
+      <c r="B242" s="17"/>
     </row>
     <row r="243" ht="15.75" customHeight="1">
-      <c r="B243" s="12"/>
+      <c r="B243" s="17"/>
     </row>
     <row r="244" ht="15.75" customHeight="1">
-      <c r="B244" s="12"/>
+      <c r="B244" s="17"/>
     </row>
     <row r="245" ht="15.75" customHeight="1">
-      <c r="B245" s="12"/>
+      <c r="B245" s="17"/>
     </row>
     <row r="246" ht="15.75" customHeight="1">
-      <c r="B246" s="12"/>
+      <c r="B246" s="17"/>
     </row>
     <row r="247" ht="15.75" customHeight="1">
-      <c r="B247" s="12"/>
+      <c r="B247" s="17"/>
     </row>
     <row r="248" ht="15.75" customHeight="1">
-      <c r="B248" s="12"/>
+      <c r="B248" s="17"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="B249" s="12"/>
+      <c r="B249" s="17"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="B250" s="12"/>
+      <c r="B250" s="17"/>
     </row>
     <row r="251" ht="15.75" customHeight="1">
-      <c r="B251" s="12"/>
+      <c r="B251" s="17"/>
     </row>
     <row r="252" ht="15.75" customHeight="1">
-      <c r="B252" s="12"/>
+      <c r="B252" s="17"/>
     </row>
     <row r="253" ht="15.75" customHeight="1">
-      <c r="B253" s="12"/>
+      <c r="B253" s="17"/>
     </row>
     <row r="254" ht="15.75" customHeight="1">
-      <c r="B254" s="12"/>
+      <c r="B254" s="17"/>
     </row>
     <row r="255" ht="15.75" customHeight="1">
-      <c r="B255" s="12"/>
+      <c r="B255" s="17"/>
     </row>
     <row r="256" ht="15.75" customHeight="1">
-      <c r="B256" s="12"/>
+      <c r="B256" s="17"/>
     </row>
     <row r="257" ht="15.75" customHeight="1">
-      <c r="B257" s="12"/>
+      <c r="B257" s="17"/>
     </row>
     <row r="258" ht="15.75" customHeight="1">
-      <c r="B258" s="12"/>
+      <c r="B258" s="17"/>
     </row>
     <row r="259" ht="15.75" customHeight="1">
-      <c r="B259" s="12"/>
+      <c r="B259" s="17"/>
     </row>
     <row r="260" ht="15.75" customHeight="1">
-      <c r="B260" s="12"/>
+      <c r="B260" s="17"/>
     </row>
     <row r="261" ht="15.75" customHeight="1">
-      <c r="B261" s="12"/>
+      <c r="B261" s="17"/>
     </row>
     <row r="262" ht="15.75" customHeight="1">
-      <c r="B262" s="12"/>
+      <c r="B262" s="17"/>
     </row>
     <row r="263" ht="15.75" customHeight="1">
-      <c r="B263" s="12"/>
+      <c r="B263" s="17"/>
     </row>
     <row r="264" ht="15.75" customHeight="1">
-      <c r="B264" s="12"/>
+      <c r="B264" s="17"/>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="B265" s="12"/>
+      <c r="B265" s="17"/>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="B266" s="12"/>
+      <c r="B266" s="17"/>
     </row>
     <row r="267" ht="15.75" customHeight="1">
-      <c r="B267" s="12"/>
+      <c r="B267" s="17"/>
     </row>
     <row r="268" ht="15.75" customHeight="1">
-      <c r="B268" s="12"/>
+      <c r="B268" s="17"/>
     </row>
     <row r="269" ht="15.75" customHeight="1">
-      <c r="B269" s="12"/>
+      <c r="B269" s="17"/>
     </row>
     <row r="270" ht="15.75" customHeight="1">
-      <c r="B270" s="12"/>
+      <c r="B270" s="17"/>
     </row>
     <row r="271" ht="15.75" customHeight="1">
-      <c r="B271" s="12"/>
+      <c r="B271" s="17"/>
     </row>
     <row r="272" ht="15.75" customHeight="1">
-      <c r="B272" s="12"/>
+      <c r="B272" s="17"/>
     </row>
     <row r="273" ht="15.75" customHeight="1">
-      <c r="B273" s="12"/>
+      <c r="B273" s="17"/>
     </row>
     <row r="274" ht="15.75" customHeight="1">
-      <c r="B274" s="12"/>
+      <c r="B274" s="17"/>
     </row>
     <row r="275" ht="15.75" customHeight="1">
-      <c r="B275" s="12"/>
+      <c r="B275" s="17"/>
     </row>
     <row r="276" ht="15.75" customHeight="1">
-      <c r="B276" s="12"/>
+      <c r="B276" s="17"/>
     </row>
     <row r="277" ht="15.75" customHeight="1">
-      <c r="B277" s="12"/>
+      <c r="B277" s="17"/>
     </row>
     <row r="278" ht="15.75" customHeight="1">
-      <c r="B278" s="12"/>
+      <c r="B278" s="17"/>
     </row>
     <row r="279" ht="15.75" customHeight="1">
-      <c r="B279" s="12"/>
+      <c r="B279" s="17"/>
     </row>
     <row r="280" ht="15.75" customHeight="1">
-      <c r="B280" s="12"/>
+      <c r="B280" s="17"/>
     </row>
     <row r="281" ht="15.75" customHeight="1">
-      <c r="B281" s="12"/>
+      <c r="B281" s="17"/>
     </row>
     <row r="282" ht="15.75" customHeight="1">
-      <c r="B282" s="12"/>
+      <c r="B282" s="17"/>
     </row>
     <row r="283" ht="15.75" customHeight="1">
-      <c r="B283" s="12"/>
+      <c r="B283" s="17"/>
     </row>
     <row r="284" ht="15.75" customHeight="1">
-      <c r="B284" s="12"/>
+      <c r="B284" s="17"/>
     </row>
     <row r="285" ht="15.75" customHeight="1">
-      <c r="B285" s="12"/>
+      <c r="B285" s="17"/>
     </row>
     <row r="286" ht="15.75" customHeight="1">
-      <c r="B286" s="12"/>
+      <c r="B286" s="17"/>
     </row>
     <row r="287" ht="15.75" customHeight="1">
-      <c r="B287" s="12"/>
+      <c r="B287" s="17"/>
     </row>
     <row r="288" ht="15.75" customHeight="1">
-      <c r="B288" s="12"/>
+      <c r="B288" s="17"/>
     </row>
     <row r="289" ht="15.75" customHeight="1">
-      <c r="B289" s="12"/>
+      <c r="B289" s="17"/>
     </row>
     <row r="290" ht="15.75" customHeight="1">
-      <c r="B290" s="12"/>
+      <c r="B290" s="17"/>
     </row>
     <row r="291" ht="15.75" customHeight="1">
-      <c r="B291" s="12"/>
+      <c r="B291" s="17"/>
     </row>
     <row r="292" ht="15.75" customHeight="1">
-      <c r="B292" s="12"/>
+      <c r="B292" s="17"/>
     </row>
     <row r="293" ht="15.75" customHeight="1">
-      <c r="B293" s="12"/>
+      <c r="B293" s="17"/>
     </row>
     <row r="294" ht="15.75" customHeight="1">
-      <c r="B294" s="12"/>
+      <c r="B294" s="17"/>
     </row>
     <row r="295" ht="15.75" customHeight="1">
-      <c r="B295" s="12"/>
+      <c r="B295" s="17"/>
     </row>
     <row r="296" ht="15.75" customHeight="1">
-      <c r="B296" s="12"/>
+      <c r="B296" s="17"/>
     </row>
     <row r="297" ht="15.75" customHeight="1">
-      <c r="B297" s="12"/>
+      <c r="B297" s="17"/>
     </row>
     <row r="298" ht="15.75" customHeight="1">
-      <c r="B298" s="12"/>
+      <c r="B298" s="17"/>
     </row>
     <row r="299" ht="15.75" customHeight="1">
-      <c r="B299" s="12"/>
+      <c r="B299" s="17"/>
     </row>
     <row r="300" ht="15.75" customHeight="1">
-      <c r="B300" s="12"/>
+      <c r="B300" s="17"/>
     </row>
     <row r="301" ht="15.75" customHeight="1">
-      <c r="B301" s="12"/>
+      <c r="B301" s="17"/>
     </row>
     <row r="302" ht="15.75" customHeight="1">
-      <c r="B302" s="12"/>
+      <c r="B302" s="17"/>
     </row>
     <row r="303" ht="15.75" customHeight="1">
-      <c r="B303" s="12"/>
+      <c r="B303" s="17"/>
     </row>
     <row r="304" ht="15.75" customHeight="1">
-      <c r="B304" s="12"/>
+      <c r="B304" s="17"/>
     </row>
     <row r="305" ht="15.75" customHeight="1">
-      <c r="B305" s="12"/>
+      <c r="B305" s="17"/>
     </row>
     <row r="306" ht="15.75" customHeight="1">
-      <c r="B306" s="12"/>
+      <c r="B306" s="17"/>
     </row>
     <row r="307" ht="15.75" customHeight="1">
-      <c r="B307" s="12"/>
+      <c r="B307" s="17"/>
     </row>
     <row r="308" ht="15.75" customHeight="1">
-      <c r="B308" s="12"/>
+      <c r="B308" s="17"/>
     </row>
     <row r="309" ht="15.75" customHeight="1">
-      <c r="B309" s="12"/>
+      <c r="B309" s="17"/>
     </row>
     <row r="310" ht="15.75" customHeight="1">
-      <c r="B310" s="12"/>
+      <c r="B310" s="17"/>
     </row>
     <row r="311" ht="15.75" customHeight="1">
-      <c r="B311" s="12"/>
+      <c r="B311" s="17"/>
     </row>
     <row r="312" ht="15.75" customHeight="1">
-      <c r="B312" s="12"/>
+      <c r="B312" s="17"/>
     </row>
     <row r="313" ht="15.75" customHeight="1">
-      <c r="B313" s="12"/>
+      <c r="B313" s="17"/>
     </row>
     <row r="314" ht="15.75" customHeight="1">
-      <c r="B314" s="12"/>
+      <c r="B314" s="17"/>
     </row>
     <row r="315" ht="15.75" customHeight="1">
-      <c r="B315" s="12"/>
+      <c r="B315" s="17"/>
     </row>
     <row r="316" ht="15.75" customHeight="1">
-      <c r="B316" s="12"/>
+      <c r="B316" s="17"/>
     </row>
     <row r="317" ht="15.75" customHeight="1">
-      <c r="B317" s="12"/>
+      <c r="B317" s="17"/>
     </row>
     <row r="318" ht="15.75" customHeight="1">
-      <c r="B318" s="12"/>
+      <c r="B318" s="17"/>
     </row>
     <row r="319" ht="15.75" customHeight="1">
-      <c r="B319" s="12"/>
+      <c r="B319" s="17"/>
     </row>
     <row r="320" ht="15.75" customHeight="1">
-      <c r="B320" s="12"/>
+      <c r="B320" s="17"/>
     </row>
     <row r="321" ht="15.75" customHeight="1">
-      <c r="B321" s="12"/>
+      <c r="B321" s="17"/>
     </row>
     <row r="322" ht="15.75" customHeight="1">
-      <c r="B322" s="12"/>
+      <c r="B322" s="17"/>
     </row>
     <row r="323" ht="15.75" customHeight="1">
-      <c r="B323" s="12"/>
+      <c r="B323" s="17"/>
     </row>
     <row r="324" ht="15.75" customHeight="1">
-      <c r="B324" s="12"/>
+      <c r="B324" s="17"/>
     </row>
     <row r="325" ht="15.75" customHeight="1">
-      <c r="B325" s="12"/>
+      <c r="B325" s="17"/>
     </row>
     <row r="326" ht="15.75" customHeight="1">
-      <c r="B326" s="12"/>
+      <c r="B326" s="17"/>
     </row>
     <row r="327" ht="15.75" customHeight="1">
-      <c r="B327" s="12"/>
+      <c r="B327" s="17"/>
     </row>
     <row r="328" ht="15.75" customHeight="1">
-      <c r="B328" s="12"/>
+      <c r="B328" s="17"/>
     </row>
     <row r="329" ht="15.75" customHeight="1">
-      <c r="B329" s="12"/>
+      <c r="B329" s="17"/>
     </row>
     <row r="330" ht="15.75" customHeight="1">
-      <c r="B330" s="12"/>
+      <c r="B330" s="17"/>
     </row>
     <row r="331" ht="15.75" customHeight="1">
-      <c r="B331" s="12"/>
+      <c r="B331" s="17"/>
     </row>
     <row r="332" ht="15.75" customHeight="1">
-      <c r="B332" s="12"/>
+      <c r="B332" s="17"/>
     </row>
     <row r="333" ht="15.75" customHeight="1">
-      <c r="B333" s="12"/>
+      <c r="B333" s="17"/>
     </row>
     <row r="334" ht="15.75" customHeight="1">
-      <c r="B334" s="12"/>
+      <c r="B334" s="17"/>
     </row>
     <row r="335" ht="15.75" customHeight="1">
-      <c r="B335" s="12"/>
+      <c r="B335" s="17"/>
     </row>
     <row r="336" ht="15.75" customHeight="1">
-      <c r="B336" s="12"/>
+      <c r="B336" s="17"/>
     </row>
     <row r="337" ht="15.75" customHeight="1">
-      <c r="B337" s="12"/>
+      <c r="B337" s="17"/>
     </row>
     <row r="338" ht="15.75" customHeight="1">
-      <c r="B338" s="12"/>
+      <c r="B338" s="17"/>
     </row>
     <row r="339" ht="15.75" customHeight="1">
-      <c r="B339" s="12"/>
+      <c r="B339" s="17"/>
     </row>
     <row r="340" ht="15.75" customHeight="1">
-      <c r="B340" s="12"/>
+      <c r="B340" s="17"/>
     </row>
     <row r="341" ht="15.75" customHeight="1">
-      <c r="B341" s="12"/>
+      <c r="B341" s="17"/>
     </row>
     <row r="342" ht="15.75" customHeight="1">
-      <c r="B342" s="12"/>
+      <c r="B342" s="17"/>
     </row>
     <row r="343" ht="15.75" customHeight="1">
-      <c r="B343" s="12"/>
+      <c r="B343" s="17"/>
     </row>
     <row r="344" ht="15.75" customHeight="1">
-      <c r="B344" s="12"/>
+      <c r="B344" s="17"/>
     </row>
     <row r="345" ht="15.75" customHeight="1">
-      <c r="B345" s="12"/>
+      <c r="B345" s="17"/>
     </row>
     <row r="346" ht="15.75" customHeight="1">
-      <c r="B346" s="12"/>
+      <c r="B346" s="17"/>
     </row>
     <row r="347" ht="15.75" customHeight="1">
-      <c r="B347" s="12"/>
+      <c r="B347" s="17"/>
     </row>
     <row r="348" ht="15.75" customHeight="1">
-      <c r="B348" s="12"/>
+      <c r="B348" s="17"/>
     </row>
     <row r="349" ht="15.75" customHeight="1">
-      <c r="B349" s="12"/>
+      <c r="B349" s="17"/>
     </row>
     <row r="350" ht="15.75" customHeight="1">
-      <c r="B350" s="12"/>
+      <c r="B350" s="17"/>
     </row>
     <row r="351" ht="15.75" customHeight="1">
-      <c r="B351" s="12"/>
+      <c r="B351" s="17"/>
     </row>
     <row r="352" ht="15.75" customHeight="1">
-      <c r="B352" s="12"/>
+      <c r="B352" s="17"/>
     </row>
     <row r="353" ht="15.75" customHeight="1">
-      <c r="B353" s="12"/>
+      <c r="B353" s="17"/>
     </row>
     <row r="354" ht="15.75" customHeight="1">
-      <c r="B354" s="12"/>
+      <c r="B354" s="17"/>
     </row>
     <row r="355" ht="15.75" customHeight="1">
-      <c r="B355" s="12"/>
+      <c r="B355" s="17"/>
     </row>
     <row r="356" ht="15.75" customHeight="1">
-      <c r="B356" s="12"/>
+      <c r="B356" s="17"/>
     </row>
     <row r="357" ht="15.75" customHeight="1">
-      <c r="B357" s="12"/>
+      <c r="B357" s="17"/>
     </row>
     <row r="358" ht="15.75" customHeight="1">
-      <c r="B358" s="12"/>
+      <c r="B358" s="17"/>
     </row>
     <row r="359" ht="15.75" customHeight="1">
-      <c r="B359" s="12"/>
+      <c r="B359" s="17"/>
     </row>
     <row r="360" ht="15.75" customHeight="1">
-      <c r="B360" s="12"/>
+      <c r="B360" s="17"/>
     </row>
     <row r="361" ht="15.75" customHeight="1">
-      <c r="B361" s="12"/>
+      <c r="B361" s="17"/>
     </row>
     <row r="362" ht="15.75" customHeight="1">
-      <c r="B362" s="12"/>
+      <c r="B362" s="17"/>
     </row>
     <row r="363" ht="15.75" customHeight="1">
-      <c r="B363" s="12"/>
+      <c r="B363" s="17"/>
     </row>
     <row r="364" ht="15.75" customHeight="1">
-      <c r="B364" s="12"/>
+      <c r="B364" s="17"/>
     </row>
     <row r="365" ht="15.75" customHeight="1">
-      <c r="B365" s="12"/>
+      <c r="B365" s="17"/>
     </row>
     <row r="366" ht="15.75" customHeight="1">
-      <c r="B366" s="12"/>
+      <c r="B366" s="17"/>
     </row>
     <row r="367" ht="15.75" customHeight="1">
-      <c r="B367" s="12"/>
+      <c r="B367" s="17"/>
     </row>
     <row r="368" ht="15.75" customHeight="1">
-      <c r="B368" s="12"/>
+      <c r="B368" s="17"/>
     </row>
     <row r="369" ht="15.75" customHeight="1">
-      <c r="B369" s="12"/>
+      <c r="B369" s="17"/>
     </row>
     <row r="370" ht="15.75" customHeight="1">
-      <c r="B370" s="12"/>
+      <c r="B370" s="17"/>
     </row>
     <row r="371" ht="15.75" customHeight="1">
-      <c r="B371" s="12"/>
+      <c r="B371" s="17"/>
     </row>
     <row r="372" ht="15.75" customHeight="1">
-      <c r="B372" s="12"/>
+      <c r="B372" s="17"/>
     </row>
     <row r="373" ht="15.75" customHeight="1">
-      <c r="B373" s="12"/>
+      <c r="B373" s="17"/>
     </row>
     <row r="374" ht="15.75" customHeight="1">
-      <c r="B374" s="12"/>
+      <c r="B374" s="17"/>
     </row>
     <row r="375" ht="15.75" customHeight="1">
-      <c r="B375" s="12"/>
+      <c r="B375" s="17"/>
     </row>
     <row r="376" ht="15.75" customHeight="1">
-      <c r="B376" s="12"/>
+      <c r="B376" s="17"/>
     </row>
     <row r="377" ht="15.75" customHeight="1">
-      <c r="B377" s="12"/>
+      <c r="B377" s="17"/>
     </row>
     <row r="378" ht="15.75" customHeight="1">
-      <c r="B378" s="12"/>
+      <c r="B378" s="17"/>
     </row>
     <row r="379" ht="15.75" customHeight="1">
-      <c r="B379" s="12"/>
+      <c r="B379" s="17"/>
     </row>
     <row r="380" ht="15.75" customHeight="1">
-      <c r="B380" s="12"/>
+      <c r="B380" s="17"/>
     </row>
     <row r="381" ht="15.75" customHeight="1">
-      <c r="B381" s="12"/>
+      <c r="B381" s="17"/>
     </row>
     <row r="382" ht="15.75" customHeight="1">
-      <c r="B382" s="12"/>
+      <c r="B382" s="17"/>
     </row>
     <row r="383" ht="15.75" customHeight="1">
-      <c r="B383" s="12"/>
+      <c r="B383" s="17"/>
     </row>
     <row r="384" ht="15.75" customHeight="1">
-      <c r="B384" s="12"/>
+      <c r="B384" s="17"/>
     </row>
     <row r="385" ht="15.75" customHeight="1">
-      <c r="B385" s="12"/>
+      <c r="B385" s="17"/>
     </row>
     <row r="386" ht="15.75" customHeight="1">
-      <c r="B386" s="12"/>
+      <c r="B386" s="17"/>
     </row>
     <row r="387" ht="15.75" customHeight="1">
-      <c r="B387" s="12"/>
+      <c r="B387" s="17"/>
     </row>
     <row r="388" ht="15.75" customHeight="1">
-      <c r="B388" s="12"/>
+      <c r="B388" s="17"/>
     </row>
     <row r="389" ht="15.75" customHeight="1">
-      <c r="B389" s="12"/>
+      <c r="B389" s="17"/>
     </row>
     <row r="390" ht="15.75" customHeight="1">
-      <c r="B390" s="12"/>
+      <c r="B390" s="17"/>
     </row>
     <row r="391" ht="15.75" customHeight="1">
-      <c r="B391" s="12"/>
+      <c r="B391" s="17"/>
     </row>
     <row r="392" ht="15.75" customHeight="1">
-      <c r="B392" s="12"/>
+      <c r="B392" s="17"/>
     </row>
     <row r="393" ht="15.75" customHeight="1">
-      <c r="B393" s="12"/>
+      <c r="B393" s="17"/>
     </row>
     <row r="394" ht="15.75" customHeight="1">
-      <c r="B394" s="12"/>
+      <c r="B394" s="17"/>
     </row>
     <row r="395" ht="15.75" customHeight="1">
-      <c r="B395" s="12"/>
+      <c r="B395" s="17"/>
     </row>
     <row r="396" ht="15.75" customHeight="1">
-      <c r="B396" s="12"/>
+      <c r="B396" s="17"/>
     </row>
     <row r="397" ht="15.75" customHeight="1">
-      <c r="B397" s="12"/>
+      <c r="B397" s="17"/>
     </row>
     <row r="398" ht="15.75" customHeight="1">
-      <c r="B398" s="12"/>
+      <c r="B398" s="17"/>
     </row>
     <row r="399" ht="15.75" customHeight="1">
-      <c r="B399" s="12"/>
+      <c r="B399" s="17"/>
     </row>
     <row r="400" ht="15.75" customHeight="1">
-      <c r="B400" s="12"/>
+      <c r="B400" s="17"/>
     </row>
     <row r="401" ht="15.75" customHeight="1">
-      <c r="B401" s="12"/>
+      <c r="B401" s="17"/>
     </row>
     <row r="402" ht="15.75" customHeight="1">
-      <c r="B402" s="12"/>
+      <c r="B402" s="17"/>
     </row>
     <row r="403" ht="15.75" customHeight="1">
-      <c r="B403" s="12"/>
+      <c r="B403" s="17"/>
     </row>
     <row r="404" ht="15.75" customHeight="1">
-      <c r="B404" s="12"/>
+      <c r="B404" s="17"/>
     </row>
     <row r="405" ht="15.75" customHeight="1">
-      <c r="B405" s="12"/>
+      <c r="B405" s="17"/>
     </row>
     <row r="406" ht="15.75" customHeight="1">
-      <c r="B406" s="12"/>
+      <c r="B406" s="17"/>
     </row>
     <row r="407" ht="15.75" customHeight="1">
-      <c r="B407" s="12"/>
+      <c r="B407" s="17"/>
     </row>
     <row r="408" ht="15.75" customHeight="1">
-      <c r="B408" s="12"/>
+      <c r="B408" s="17"/>
     </row>
     <row r="409" ht="15.75" customHeight="1">
-      <c r="B409" s="12"/>
+      <c r="B409" s="17"/>
     </row>
     <row r="410" ht="15.75" customHeight="1">
-      <c r="B410" s="12"/>
+      <c r="B410" s="17"/>
     </row>
     <row r="411" ht="15.75" customHeight="1">
-      <c r="B411" s="12"/>
+      <c r="B411" s="17"/>
     </row>
     <row r="412" ht="15.75" customHeight="1">
-      <c r="B412" s="12"/>
+      <c r="B412" s="17"/>
     </row>
     <row r="413" ht="15.75" customHeight="1">
-      <c r="B413" s="12"/>
+      <c r="B413" s="17"/>
     </row>
     <row r="414" ht="15.75" customHeight="1">
-      <c r="B414" s="12"/>
+      <c r="B414" s="17"/>
     </row>
     <row r="415" ht="15.75" customHeight="1">
-      <c r="B415" s="12"/>
+      <c r="B415" s="17"/>
     </row>
     <row r="416" ht="15.75" customHeight="1">
-      <c r="B416" s="12"/>
+      <c r="B416" s="17"/>
     </row>
     <row r="417" ht="15.75" customHeight="1">
-      <c r="B417" s="12"/>
+      <c r="B417" s="17"/>
     </row>
     <row r="418" ht="15.75" customHeight="1">
-      <c r="B418" s="12"/>
+      <c r="B418" s="17"/>
     </row>
     <row r="419" ht="15.75" customHeight="1">
-      <c r="B419" s="12"/>
+      <c r="B419" s="17"/>
     </row>
     <row r="420" ht="15.75" customHeight="1">
-      <c r="B420" s="12"/>
+      <c r="B420" s="17"/>
     </row>
     <row r="421" ht="15.75" customHeight="1">
-      <c r="B421" s="12"/>
+      <c r="B421" s="17"/>
     </row>
     <row r="422" ht="15.75" customHeight="1">
-      <c r="B422" s="12"/>
+      <c r="B422" s="17"/>
     </row>
     <row r="423" ht="15.75" customHeight="1">
-      <c r="B423" s="12"/>
+      <c r="B423" s="17"/>
     </row>
     <row r="424" ht="15.75" customHeight="1">
-      <c r="B424" s="12"/>
+      <c r="B424" s="17"/>
     </row>
     <row r="425" ht="15.75" customHeight="1">
-      <c r="B425" s="12"/>
+      <c r="B425" s="17"/>
     </row>
     <row r="426" ht="15.75" customHeight="1">
-      <c r="B426" s="12"/>
+      <c r="B426" s="17"/>
     </row>
     <row r="427" ht="15.75" customHeight="1">
-      <c r="B427" s="12"/>
+      <c r="B427" s="17"/>
     </row>
     <row r="428" ht="15.75" customHeight="1">
-      <c r="B428" s="12"/>
+      <c r="B428" s="17"/>
     </row>
     <row r="429" ht="15.75" customHeight="1">
-      <c r="B429" s="12"/>
+      <c r="B429" s="17"/>
     </row>
     <row r="430" ht="15.75" customHeight="1">
-      <c r="B430" s="12"/>
+      <c r="B430" s="17"/>
     </row>
     <row r="431" ht="15.75" customHeight="1">
-      <c r="B431" s="12"/>
+      <c r="B431" s="17"/>
     </row>
     <row r="432" ht="15.75" customHeight="1">
-      <c r="B432" s="12"/>
+      <c r="B432" s="17"/>
     </row>
     <row r="433" ht="15.75" customHeight="1">
-      <c r="B433" s="12"/>
+      <c r="B433" s="17"/>
     </row>
     <row r="434" ht="15.75" customHeight="1">
-      <c r="B434" s="12"/>
+      <c r="B434" s="17"/>
     </row>
     <row r="435" ht="15.75" customHeight="1">
-      <c r="B435" s="12"/>
+      <c r="B435" s="17"/>
     </row>
     <row r="436" ht="15.75" customHeight="1">
-      <c r="B436" s="12"/>
+      <c r="B436" s="17"/>
     </row>
     <row r="437" ht="15.75" customHeight="1">
-      <c r="B437" s="12"/>
+      <c r="B437" s="17"/>
     </row>
     <row r="438" ht="15.75" customHeight="1">
-      <c r="B438" s="12"/>
+      <c r="B438" s="17"/>
     </row>
     <row r="439" ht="15.75" customHeight="1">
-      <c r="B439" s="12"/>
+      <c r="B439" s="17"/>
     </row>
     <row r="440" ht="15.75" customHeight="1">
-      <c r="B440" s="12"/>
+      <c r="B440" s="17"/>
     </row>
     <row r="441" ht="15.75" customHeight="1">
-      <c r="B441" s="12"/>
+      <c r="B441" s="17"/>
     </row>
     <row r="442" ht="15.75" customHeight="1">
-      <c r="B442" s="12"/>
+      <c r="B442" s="17"/>
     </row>
     <row r="443" ht="15.75" customHeight="1">
-      <c r="B443" s="12"/>
+      <c r="B443" s="17"/>
     </row>
     <row r="444" ht="15.75" customHeight="1">
-      <c r="B444" s="12"/>
+      <c r="B444" s="17"/>
     </row>
     <row r="445" ht="15.75" customHeight="1">
-      <c r="B445" s="12"/>
+      <c r="B445" s="17"/>
     </row>
     <row r="446" ht="15.75" customHeight="1">
-      <c r="B446" s="12"/>
+      <c r="B446" s="17"/>
     </row>
     <row r="447" ht="15.75" customHeight="1">
-      <c r="B447" s="12"/>
+      <c r="B447" s="17"/>
     </row>
     <row r="448" ht="15.75" customHeight="1">
-      <c r="B448" s="12"/>
+      <c r="B448" s="17"/>
     </row>
     <row r="449" ht="15.75" customHeight="1">
-      <c r="B449" s="12"/>
+      <c r="B449" s="17"/>
     </row>
     <row r="450" ht="15.75" customHeight="1">
-      <c r="B450" s="12"/>
+      <c r="B450" s="17"/>
     </row>
     <row r="451" ht="15.75" customHeight="1">
-      <c r="B451" s="12"/>
+      <c r="B451" s="17"/>
     </row>
     <row r="452" ht="15.75" customHeight="1">
-      <c r="B452" s="12"/>
+      <c r="B452" s="17"/>
     </row>
     <row r="453" ht="15.75" customHeight="1">
-      <c r="B453" s="12"/>
+      <c r="B453" s="17"/>
     </row>
     <row r="454" ht="15.75" customHeight="1">
-      <c r="B454" s="12"/>
+      <c r="B454" s="17"/>
     </row>
     <row r="455" ht="15.75" customHeight="1">
-      <c r="B455" s="12"/>
+      <c r="B455" s="17"/>
     </row>
     <row r="456" ht="15.75" customHeight="1">
-      <c r="B456" s="12"/>
+      <c r="B456" s="17"/>
     </row>
     <row r="457" ht="15.75" customHeight="1">
-      <c r="B457" s="12"/>
+      <c r="B457" s="17"/>
     </row>
     <row r="458" ht="15.75" customHeight="1">
-      <c r="B458" s="12"/>
+      <c r="B458" s="17"/>
     </row>
     <row r="459" ht="15.75" customHeight="1">
-      <c r="B459" s="12"/>
+      <c r="B459" s="17"/>
     </row>
     <row r="460" ht="15.75" customHeight="1">
-      <c r="B460" s="12"/>
+      <c r="B460" s="17"/>
     </row>
     <row r="461" ht="15.75" customHeight="1">
-      <c r="B461" s="12"/>
+      <c r="B461" s="17"/>
     </row>
     <row r="462" ht="15.75" customHeight="1">
-      <c r="B462" s="12"/>
+      <c r="B462" s="17"/>
     </row>
     <row r="463" ht="15.75" customHeight="1">
-      <c r="B463" s="12"/>
+      <c r="B463" s="17"/>
     </row>
     <row r="464" ht="15.75" customHeight="1">
-      <c r="B464" s="12"/>
+      <c r="B464" s="17"/>
     </row>
     <row r="465" ht="15.75" customHeight="1">
-      <c r="B465" s="12"/>
+      <c r="B465" s="17"/>
     </row>
     <row r="466" ht="15.75" customHeight="1">
-      <c r="B466" s="12"/>
+      <c r="B466" s="17"/>
     </row>
     <row r="467" ht="15.75" customHeight="1">
-      <c r="B467" s="12"/>
+      <c r="B467" s="17"/>
     </row>
     <row r="468" ht="15.75" customHeight="1">
-      <c r="B468" s="12"/>
+      <c r="B468" s="17"/>
     </row>
     <row r="469" ht="15.75" customHeight="1">
-      <c r="B469" s="12"/>
+      <c r="B469" s="17"/>
     </row>
     <row r="470" ht="15.75" customHeight="1">
-      <c r="B470" s="12"/>
+      <c r="B470" s="17"/>
     </row>
     <row r="471" ht="15.75" customHeight="1">
-      <c r="B471" s="12"/>
+      <c r="B471" s="17"/>
     </row>
     <row r="472" ht="15.75" customHeight="1">
-      <c r="B472" s="12"/>
+      <c r="B472" s="17"/>
     </row>
     <row r="473" ht="15.75" customHeight="1">
-      <c r="B473" s="12"/>
+      <c r="B473" s="17"/>
     </row>
     <row r="474" ht="15.75" customHeight="1">
-      <c r="B474" s="12"/>
+      <c r="B474" s="17"/>
     </row>
     <row r="475" ht="15.75" customHeight="1">
-      <c r="B475" s="12"/>
+      <c r="B475" s="17"/>
     </row>
     <row r="476" ht="15.75" customHeight="1">
-      <c r="B476" s="12"/>
+      <c r="B476" s="17"/>
     </row>
     <row r="477" ht="15.75" customHeight="1">
-      <c r="B477" s="12"/>
+      <c r="B477" s="17"/>
     </row>
     <row r="478" ht="15.75" customHeight="1">
-      <c r="B478" s="12"/>
+      <c r="B478" s="17"/>
     </row>
     <row r="479" ht="15.75" customHeight="1">
-      <c r="B479" s="12"/>
+      <c r="B479" s="17"/>
     </row>
     <row r="480" ht="15.75" customHeight="1">
-      <c r="B480" s="12"/>
+      <c r="B480" s="17"/>
     </row>
     <row r="481" ht="15.75" customHeight="1">
-      <c r="B481" s="12"/>
+      <c r="B481" s="17"/>
     </row>
     <row r="482" ht="15.75" customHeight="1">
-      <c r="B482" s="12"/>
+      <c r="B482" s="17"/>
     </row>
     <row r="483" ht="15.75" customHeight="1">
-      <c r="B483" s="12"/>
+      <c r="B483" s="17"/>
     </row>
     <row r="484" ht="15.75" customHeight="1">
-      <c r="B484" s="12"/>
+      <c r="B484" s="17"/>
     </row>
     <row r="485" ht="15.75" customHeight="1">
-      <c r="B485" s="12"/>
+      <c r="B485" s="17"/>
     </row>
     <row r="486" ht="15.75" customHeight="1">
-      <c r="B486" s="12"/>
+      <c r="B486" s="17"/>
     </row>
     <row r="487" ht="15.75" customHeight="1">
-      <c r="B487" s="12"/>
+      <c r="B487" s="17"/>
     </row>
     <row r="488" ht="15.75" customHeight="1">
-      <c r="B488" s="12"/>
+      <c r="B488" s="17"/>
     </row>
     <row r="489" ht="15.75" customHeight="1">
-      <c r="B489" s="12"/>
+      <c r="B489" s="17"/>
     </row>
     <row r="490" ht="15.75" customHeight="1">
-      <c r="B490" s="12"/>
+      <c r="B490" s="17"/>
     </row>
     <row r="491" ht="15.75" customHeight="1">
-      <c r="B491" s="12"/>
+      <c r="B491" s="17"/>
     </row>
     <row r="492" ht="15.75" customHeight="1">
-      <c r="B492" s="12"/>
+      <c r="B492" s="17"/>
     </row>
     <row r="493" ht="15.75" customHeight="1">
-      <c r="B493" s="12"/>
+      <c r="B493" s="17"/>
     </row>
     <row r="494" ht="15.75" customHeight="1">
-      <c r="B494" s="12"/>
+      <c r="B494" s="17"/>
     </row>
     <row r="495" ht="15.75" customHeight="1">
-      <c r="B495" s="12"/>
+      <c r="B495" s="17"/>
     </row>
     <row r="496" ht="15.75" customHeight="1">
-      <c r="B496" s="12"/>
+      <c r="B496" s="17"/>
     </row>
     <row r="497" ht="15.75" customHeight="1">
-      <c r="B497" s="12"/>
+      <c r="B497" s="17"/>
     </row>
     <row r="498" ht="15.75" customHeight="1">
-      <c r="B498" s="12"/>
+      <c r="B498" s="17"/>
     </row>
     <row r="499" ht="15.75" customHeight="1">
-      <c r="B499" s="12"/>
+      <c r="B499" s="17"/>
     </row>
     <row r="500" ht="15.75" customHeight="1">
-      <c r="B500" s="12"/>
+      <c r="B500" s="17"/>
     </row>
     <row r="501" ht="15.75" customHeight="1">
-      <c r="B501" s="12"/>
+      <c r="B501" s="17"/>
     </row>
     <row r="502" ht="15.75" customHeight="1">
-      <c r="B502" s="12"/>
+      <c r="B502" s="17"/>
     </row>
     <row r="503" ht="15.75" customHeight="1">
-      <c r="B503" s="12"/>
+      <c r="B503" s="17"/>
     </row>
     <row r="504" ht="15.75" customHeight="1">
-      <c r="B504" s="12"/>
+      <c r="B504" s="17"/>
     </row>
     <row r="505" ht="15.75" customHeight="1">
-      <c r="B505" s="12"/>
+      <c r="B505" s="17"/>
     </row>
     <row r="506" ht="15.75" customHeight="1">
-      <c r="B506" s="12"/>
+      <c r="B506" s="17"/>
     </row>
     <row r="507" ht="15.75" customHeight="1">
-      <c r="B507" s="12"/>
+      <c r="B507" s="17"/>
     </row>
     <row r="508" ht="15.75" customHeight="1">
-      <c r="B508" s="12"/>
+      <c r="B508" s="17"/>
     </row>
     <row r="509" ht="15.75" customHeight="1">
-      <c r="B509" s="12"/>
+      <c r="B509" s="17"/>
     </row>
     <row r="510" ht="15.75" customHeight="1">
-      <c r="B510" s="12"/>
+      <c r="B510" s="17"/>
     </row>
     <row r="511" ht="15.75" customHeight="1">
-      <c r="B511" s="12"/>
+      <c r="B511" s="17"/>
     </row>
     <row r="512" ht="15.75" customHeight="1">
-      <c r="B512" s="12"/>
+      <c r="B512" s="17"/>
     </row>
     <row r="513" ht="15.75" customHeight="1">
-      <c r="B513" s="12"/>
+      <c r="B513" s="17"/>
     </row>
     <row r="514" ht="15.75" customHeight="1">
-      <c r="B514" s="12"/>
+      <c r="B514" s="17"/>
     </row>
     <row r="515" ht="15.75" customHeight="1">
-      <c r="B515" s="12"/>
+      <c r="B515" s="17"/>
     </row>
     <row r="516" ht="15.75" customHeight="1">
-      <c r="B516" s="12"/>
+      <c r="B516" s="17"/>
     </row>
     <row r="517" ht="15.75" customHeight="1">
-      <c r="B517" s="12"/>
+      <c r="B517" s="17"/>
     </row>
     <row r="518" ht="15.75" customHeight="1">
-      <c r="B518" s="12"/>
+      <c r="B518" s="17"/>
     </row>
     <row r="519" ht="15.75" customHeight="1">
-      <c r="B519" s="12"/>
+      <c r="B519" s="17"/>
     </row>
     <row r="520" ht="15.75" customHeight="1">
-      <c r="B520" s="12"/>
+      <c r="B520" s="17"/>
     </row>
     <row r="521" ht="15.75" customHeight="1">
-      <c r="B521" s="12"/>
+      <c r="B521" s="17"/>
     </row>
     <row r="522" ht="15.75" customHeight="1">
-      <c r="B522" s="12"/>
+      <c r="B522" s="17"/>
     </row>
     <row r="523" ht="15.75" customHeight="1">
-      <c r="B523" s="12"/>
+      <c r="B523" s="17"/>
     </row>
     <row r="524" ht="15.75" customHeight="1">
-      <c r="B524" s="12"/>
+      <c r="B524" s="17"/>
     </row>
     <row r="525" ht="15.75" customHeight="1">
-      <c r="B525" s="12"/>
+      <c r="B525" s="17"/>
     </row>
     <row r="526" ht="15.75" customHeight="1">
-      <c r="B526" s="12"/>
+      <c r="B526" s="17"/>
     </row>
     <row r="527" ht="15.75" customHeight="1">
-      <c r="B527" s="12"/>
+      <c r="B527" s="17"/>
     </row>
     <row r="528" ht="15.75" customHeight="1">
-      <c r="B528" s="12"/>
+      <c r="B528" s="17"/>
     </row>
     <row r="529" ht="15.75" customHeight="1">
-      <c r="B529" s="12"/>
+      <c r="B529" s="17"/>
     </row>
     <row r="530" ht="15.75" customHeight="1">
-      <c r="B530" s="12"/>
+      <c r="B530" s="17"/>
     </row>
     <row r="531" ht="15.75" customHeight="1">
-      <c r="B531" s="12"/>
+      <c r="B531" s="17"/>
     </row>
     <row r="532" ht="15.75" customHeight="1">
-      <c r="B532" s="12"/>
+      <c r="B532" s="17"/>
     </row>
     <row r="533" ht="15.75" customHeight="1">
-      <c r="B533" s="12"/>
+      <c r="B533" s="17"/>
     </row>
     <row r="534" ht="15.75" customHeight="1">
-      <c r="B534" s="12"/>
+      <c r="B534" s="17"/>
     </row>
     <row r="535" ht="15.75" customHeight="1">
-      <c r="B535" s="12"/>
+      <c r="B535" s="17"/>
     </row>
     <row r="536" ht="15.75" customHeight="1">
-      <c r="B536" s="12"/>
+      <c r="B536" s="17"/>
     </row>
     <row r="537" ht="15.75" customHeight="1">
-      <c r="B537" s="12"/>
+      <c r="B537" s="17"/>
     </row>
     <row r="538" ht="15.75" customHeight="1">
-      <c r="B538" s="12"/>
+      <c r="B538" s="17"/>
     </row>
     <row r="539" ht="15.75" customHeight="1">
-      <c r="B539" s="12"/>
+      <c r="B539" s="17"/>
     </row>
     <row r="540" ht="15.75" customHeight="1">
-      <c r="B540" s="12"/>
+      <c r="B540" s="17"/>
     </row>
     <row r="541" ht="15.75" customHeight="1">
-      <c r="B541" s="12"/>
+      <c r="B541" s="17"/>
     </row>
     <row r="542" ht="15.75" customHeight="1">
-      <c r="B542" s="12"/>
+      <c r="B542" s="17"/>
     </row>
     <row r="543" ht="15.75" customHeight="1">
-      <c r="B543" s="12"/>
+      <c r="B543" s="17"/>
     </row>
     <row r="544" ht="15.75" customHeight="1">
-      <c r="B544" s="12"/>
+      <c r="B544" s="17"/>
     </row>
     <row r="545" ht="15.75" customHeight="1">
-      <c r="B545" s="12"/>
+      <c r="B545" s="17"/>
     </row>
     <row r="546" ht="15.75" customHeight="1">
-      <c r="B546" s="12"/>
+      <c r="B546" s="17"/>
     </row>
     <row r="547" ht="15.75" customHeight="1">
-      <c r="B547" s="12"/>
+      <c r="B547" s="17"/>
     </row>
     <row r="548" ht="15.75" customHeight="1">
-      <c r="B548" s="12"/>
+      <c r="B548" s="17"/>
     </row>
     <row r="549" ht="15.75" customHeight="1">
-      <c r="B549" s="12"/>
+      <c r="B549" s="17"/>
     </row>
     <row r="550" ht="15.75" customHeight="1">
-      <c r="B550" s="12"/>
+      <c r="B550" s="17"/>
     </row>
     <row r="551" ht="15.75" customHeight="1">
-      <c r="B551" s="12"/>
+      <c r="B551" s="17"/>
     </row>
     <row r="552" ht="15.75" customHeight="1">
-      <c r="B552" s="12"/>
+      <c r="B552" s="17"/>
     </row>
     <row r="553" ht="15.75" customHeight="1">
-      <c r="B553" s="12"/>
+      <c r="B553" s="17"/>
     </row>
     <row r="554" ht="15.75" customHeight="1">
-      <c r="B554" s="12"/>
+      <c r="B554" s="17"/>
     </row>
     <row r="555" ht="15.75" customHeight="1">
-      <c r="B555" s="12"/>
+      <c r="B555" s="17"/>
     </row>
     <row r="556" ht="15.75" customHeight="1">
-      <c r="B556" s="12"/>
+      <c r="B556" s="17"/>
     </row>
     <row r="557" ht="15.75" customHeight="1">
-      <c r="B557" s="12"/>
+      <c r="B557" s="17"/>
     </row>
     <row r="558" ht="15.75" customHeight="1">
-      <c r="B558" s="12"/>
+      <c r="B558" s="17"/>
     </row>
     <row r="559" ht="15.75" customHeight="1">
-      <c r="B559" s="12"/>
+      <c r="B559" s="17"/>
     </row>
     <row r="560" ht="15.75" customHeight="1">
-      <c r="B560" s="12"/>
+      <c r="B560" s="17"/>
     </row>
     <row r="561" ht="15.75" customHeight="1">
-      <c r="B561" s="12"/>
+      <c r="B561" s="17"/>
     </row>
     <row r="562" ht="15.75" customHeight="1">
-      <c r="B562" s="12"/>
+      <c r="B562" s="17"/>
     </row>
     <row r="563" ht="15.75" customHeight="1">
-      <c r="B563" s="12"/>
+      <c r="B563" s="17"/>
     </row>
     <row r="564" ht="15.75" customHeight="1">
-      <c r="B564" s="12"/>
+      <c r="B564" s="17"/>
     </row>
     <row r="565" ht="15.75" customHeight="1">
-      <c r="B565" s="12"/>
+      <c r="B565" s="17"/>
     </row>
     <row r="566" ht="15.75" customHeight="1">
-      <c r="B566" s="12"/>
+      <c r="B566" s="17"/>
     </row>
     <row r="567" ht="15.75" customHeight="1">
-      <c r="B567" s="12"/>
+      <c r="B567" s="17"/>
     </row>
     <row r="568" ht="15.75" customHeight="1">
-      <c r="B568" s="12"/>
+      <c r="B568" s="17"/>
     </row>
     <row r="569" ht="15.75" customHeight="1">
-      <c r="B569" s="12"/>
+      <c r="B569" s="17"/>
     </row>
     <row r="570" ht="15.75" customHeight="1">
-      <c r="B570" s="12"/>
+      <c r="B570" s="17"/>
     </row>
     <row r="571" ht="15.75" customHeight="1">
-      <c r="B571" s="12"/>
+      <c r="B571" s="17"/>
     </row>
     <row r="572" ht="15.75" customHeight="1">
-      <c r="B572" s="12"/>
+      <c r="B572" s="17"/>
     </row>
     <row r="573" ht="15.75" customHeight="1">
-      <c r="B573" s="12"/>
+      <c r="B573" s="17"/>
     </row>
     <row r="574" ht="15.75" customHeight="1">
-      <c r="B574" s="12"/>
+      <c r="B574" s="17"/>
     </row>
     <row r="575" ht="15.75" customHeight="1">
-      <c r="B575" s="12"/>
+      <c r="B575" s="17"/>
     </row>
     <row r="576" ht="15.75" customHeight="1">
-      <c r="B576" s="12"/>
+      <c r="B576" s="17"/>
     </row>
     <row r="577" ht="15.75" customHeight="1">
-      <c r="B577" s="12"/>
+      <c r="B577" s="17"/>
     </row>
     <row r="578" ht="15.75" customHeight="1">
-      <c r="B578" s="12"/>
+      <c r="B578" s="17"/>
     </row>
     <row r="579" ht="15.75" customHeight="1">
-      <c r="B579" s="12"/>
+      <c r="B579" s="17"/>
     </row>
     <row r="580" ht="15.75" customHeight="1">
-      <c r="B580" s="12"/>
+      <c r="B580" s="17"/>
     </row>
     <row r="581" ht="15.75" customHeight="1">
-      <c r="B581" s="12"/>
+      <c r="B581" s="17"/>
     </row>
     <row r="582" ht="15.75" customHeight="1">
-      <c r="B582" s="12"/>
+      <c r="B582" s="17"/>
     </row>
     <row r="583" ht="15.75" customHeight="1">
-      <c r="B583" s="12"/>
+      <c r="B583" s="17"/>
     </row>
     <row r="584" ht="15.75" customHeight="1">
-      <c r="B584" s="12"/>
+      <c r="B584" s="17"/>
     </row>
     <row r="585" ht="15.75" customHeight="1">
-      <c r="B585" s="12"/>
+      <c r="B585" s="17"/>
     </row>
     <row r="586" ht="15.75" customHeight="1">
-      <c r="B586" s="12"/>
+      <c r="B586" s="17"/>
     </row>
     <row r="587" ht="15.75" customHeight="1">
-      <c r="B587" s="12"/>
+      <c r="B587" s="17"/>
     </row>
     <row r="588" ht="15.75" customHeight="1">
-      <c r="B588" s="12"/>
+      <c r="B588" s="17"/>
     </row>
     <row r="589" ht="15.75" customHeight="1">
-      <c r="B589" s="12"/>
+      <c r="B589" s="17"/>
     </row>
     <row r="590" ht="15.75" customHeight="1">
-      <c r="B590" s="12"/>
+      <c r="B590" s="17"/>
     </row>
     <row r="591" ht="15.75" customHeight="1">
-      <c r="B591" s="12"/>
+      <c r="B591" s="17"/>
     </row>
     <row r="592" ht="15.75" customHeight="1">
-      <c r="B592" s="12"/>
+      <c r="B592" s="17"/>
     </row>
     <row r="593" ht="15.75" customHeight="1">
-      <c r="B593" s="12"/>
+      <c r="B593" s="17"/>
     </row>
     <row r="594" ht="15.75" customHeight="1">
-      <c r="B594" s="12"/>
+      <c r="B594" s="17"/>
     </row>
     <row r="595" ht="15.75" customHeight="1">
-      <c r="B595" s="12"/>
+      <c r="B595" s="17"/>
     </row>
     <row r="596" ht="15.75" customHeight="1">
-      <c r="B596" s="12"/>
+      <c r="B596" s="17"/>
     </row>
     <row r="597" ht="15.75" customHeight="1">
-      <c r="B597" s="12"/>
+      <c r="B597" s="17"/>
     </row>
     <row r="598" ht="15.75" customHeight="1">
-      <c r="B598" s="12"/>
+      <c r="B598" s="17"/>
     </row>
     <row r="599" ht="15.75" customHeight="1">
-      <c r="B599" s="12"/>
+      <c r="B599" s="17"/>
     </row>
     <row r="600" ht="15.75" customHeight="1">
-      <c r="B600" s="12"/>
+      <c r="B600" s="17"/>
     </row>
     <row r="601" ht="15.75" customHeight="1">
-      <c r="B601" s="12"/>
+      <c r="B601" s="17"/>
     </row>
     <row r="602" ht="15.75" customHeight="1">
-      <c r="B602" s="12"/>
+      <c r="B602" s="17"/>
     </row>
     <row r="603" ht="15.75" customHeight="1">
-      <c r="B603" s="12"/>
+      <c r="B603" s="17"/>
     </row>
     <row r="604" ht="15.75" customHeight="1">
-      <c r="B604" s="12"/>
+      <c r="B604" s="17"/>
     </row>
     <row r="605" ht="15.75" customHeight="1">
-      <c r="B605" s="12"/>
+      <c r="B605" s="17"/>
     </row>
     <row r="606" ht="15.75" customHeight="1">
-      <c r="B606" s="12"/>
+      <c r="B606" s="17"/>
     </row>
     <row r="607" ht="15.75" customHeight="1">
-      <c r="B607" s="12"/>
+      <c r="B607" s="17"/>
     </row>
     <row r="608" ht="15.75" customHeight="1">
-      <c r="B608" s="12"/>
+      <c r="B608" s="17"/>
     </row>
     <row r="609" ht="15.75" customHeight="1">
-      <c r="B609" s="12"/>
+      <c r="B609" s="17"/>
     </row>
     <row r="610" ht="15.75" customHeight="1">
-      <c r="B610" s="12"/>
+      <c r="B610" s="17"/>
     </row>
     <row r="611" ht="15.75" customHeight="1">
-      <c r="B611" s="12"/>
+      <c r="B611" s="17"/>
     </row>
     <row r="612" ht="15.75" customHeight="1">
-      <c r="B612" s="12"/>
+      <c r="B612" s="17"/>
     </row>
     <row r="613" ht="15.75" customHeight="1">
-      <c r="B613" s="12"/>
+      <c r="B613" s="17"/>
     </row>
     <row r="614" ht="15.75" customHeight="1">
-      <c r="B614" s="12"/>
+      <c r="B614" s="17"/>
     </row>
     <row r="615" ht="15.75" customHeight="1">
-      <c r="B615" s="12"/>
+      <c r="B615" s="17"/>
     </row>
     <row r="616" ht="15.75" customHeight="1">
-      <c r="B616" s="12"/>
+      <c r="B616" s="17"/>
     </row>
     <row r="617" ht="15.75" customHeight="1">
-      <c r="B617" s="12"/>
+      <c r="B617" s="17"/>
     </row>
     <row r="618" ht="15.75" customHeight="1">
-      <c r="B618" s="12"/>
+      <c r="B618" s="17"/>
     </row>
     <row r="619" ht="15.75" customHeight="1">
-      <c r="B619" s="12"/>
+      <c r="B619" s="17"/>
     </row>
     <row r="620" ht="15.75" customHeight="1">
-      <c r="B620" s="12"/>
+      <c r="B620" s="17"/>
     </row>
     <row r="621" ht="15.75" customHeight="1">
-      <c r="B621" s="12"/>
+      <c r="B621" s="17"/>
     </row>
     <row r="622" ht="15.75" customHeight="1">
-      <c r="B622" s="12"/>
+      <c r="B622" s="17"/>
     </row>
     <row r="623" ht="15.75" customHeight="1">
-      <c r="B623" s="12"/>
+      <c r="B623" s="17"/>
     </row>
     <row r="624" ht="15.75" customHeight="1">
-      <c r="B624" s="12"/>
+      <c r="B624" s="17"/>
     </row>
     <row r="625" ht="15.75" customHeight="1">
-      <c r="B625" s="12"/>
+      <c r="B625" s="17"/>
     </row>
     <row r="626" ht="15.75" customHeight="1">
-      <c r="B626" s="12"/>
+      <c r="B626" s="17"/>
     </row>
     <row r="627" ht="15.75" customHeight="1">
-      <c r="B627" s="12"/>
+      <c r="B627" s="17"/>
     </row>
     <row r="628" ht="15.75" customHeight="1">
-      <c r="B628" s="12"/>
+      <c r="B628" s="17"/>
     </row>
     <row r="629" ht="15.75" customHeight="1">
-      <c r="B629" s="12"/>
+      <c r="B629" s="17"/>
     </row>
     <row r="630" ht="15.75" customHeight="1">
-      <c r="B630" s="12"/>
+      <c r="B630" s="17"/>
     </row>
     <row r="631" ht="15.75" customHeight="1">
-      <c r="B631" s="12"/>
+      <c r="B631" s="17"/>
     </row>
     <row r="632" ht="15.75" customHeight="1">
-      <c r="B632" s="12"/>
+      <c r="B632" s="17"/>
     </row>
     <row r="633" ht="15.75" customHeight="1">
-      <c r="B633" s="12"/>
+      <c r="B633" s="17"/>
     </row>
     <row r="634" ht="15.75" customHeight="1">
-      <c r="B634" s="12"/>
+      <c r="B634" s="17"/>
     </row>
     <row r="635" ht="15.75" customHeight="1">
-      <c r="B635" s="12"/>
+      <c r="B635" s="17"/>
     </row>
     <row r="636" ht="15.75" customHeight="1">
-      <c r="B636" s="12"/>
+      <c r="B636" s="17"/>
     </row>
     <row r="637" ht="15.75" customHeight="1">
-      <c r="B637" s="12"/>
+      <c r="B637" s="17"/>
     </row>
     <row r="638" ht="15.75" customHeight="1">
-      <c r="B638" s="12"/>
+      <c r="B638" s="17"/>
     </row>
     <row r="639" ht="15.75" customHeight="1">
-      <c r="B639" s="12"/>
+      <c r="B639" s="17"/>
     </row>
     <row r="640" ht="15.75" customHeight="1">
-      <c r="B640" s="12"/>
+      <c r="B640" s="17"/>
     </row>
     <row r="641" ht="15.75" customHeight="1">
-      <c r="B641" s="12"/>
+      <c r="B641" s="17"/>
     </row>
     <row r="642" ht="15.75" customHeight="1">
-      <c r="B642" s="12"/>
+      <c r="B642" s="17"/>
     </row>
     <row r="643" ht="15.75" customHeight="1">
-      <c r="B643" s="12"/>
+      <c r="B643" s="17"/>
     </row>
     <row r="644" ht="15.75" customHeight="1">
-      <c r="B644" s="12"/>
+      <c r="B644" s="17"/>
     </row>
     <row r="645" ht="15.75" customHeight="1">
-      <c r="B645" s="12"/>
+      <c r="B645" s="17"/>
     </row>
     <row r="646" ht="15.75" customHeight="1">
-      <c r="B646" s="12"/>
+      <c r="B646" s="17"/>
     </row>
     <row r="647" ht="15.75" customHeight="1">
-      <c r="B647" s="12"/>
+      <c r="B647" s="17"/>
     </row>
     <row r="648" ht="15.75" customHeight="1">
-      <c r="B648" s="12"/>
+      <c r="B648" s="17"/>
     </row>
     <row r="649" ht="15.75" customHeight="1">
-      <c r="B649" s="12"/>
+      <c r="B649" s="17"/>
     </row>
     <row r="650" ht="15.75" customHeight="1">
-      <c r="B650" s="12"/>
+      <c r="B650" s="17"/>
     </row>
     <row r="651" ht="15.75" customHeight="1">
-      <c r="B651" s="12"/>
+      <c r="B651" s="17"/>
     </row>
     <row r="652" ht="15.75" customHeight="1">
-      <c r="B652" s="12"/>
+      <c r="B652" s="17"/>
     </row>
     <row r="653" ht="15.75" customHeight="1">
-      <c r="B653" s="12"/>
+      <c r="B653" s="17"/>
     </row>
     <row r="654" ht="15.75" customHeight="1">
-      <c r="B654" s="12"/>
+      <c r="B654" s="17"/>
     </row>
     <row r="655" ht="15.75" customHeight="1">
-      <c r="B655" s="12"/>
+      <c r="B655" s="17"/>
     </row>
     <row r="656" ht="15.75" customHeight="1">
-      <c r="B656" s="12"/>
+      <c r="B656" s="17"/>
     </row>
     <row r="657" ht="15.75" customHeight="1">
-      <c r="B657" s="12"/>
+      <c r="B657" s="17"/>
     </row>
     <row r="658" ht="15.75" customHeight="1">
-      <c r="B658" s="12"/>
+      <c r="B658" s="17"/>
     </row>
     <row r="659" ht="15.75" customHeight="1">
-      <c r="B659" s="12"/>
+      <c r="B659" s="17"/>
     </row>
     <row r="660" ht="15.75" customHeight="1">
-      <c r="B660" s="12"/>
+      <c r="B660" s="17"/>
     </row>
     <row r="661" ht="15.75" customHeight="1">
-      <c r="B661" s="12"/>
+      <c r="B661" s="17"/>
     </row>
     <row r="662" ht="15.75" customHeight="1">
-      <c r="B662" s="12"/>
+      <c r="B662" s="17"/>
     </row>
     <row r="663" ht="15.75" customHeight="1">
-      <c r="B663" s="12"/>
+      <c r="B663" s="17"/>
     </row>
     <row r="664" ht="15.75" customHeight="1">
-      <c r="B664" s="12"/>
+      <c r="B664" s="17"/>
     </row>
     <row r="665" ht="15.75" customHeight="1">
-      <c r="B665" s="12"/>
+      <c r="B665" s="17"/>
     </row>
     <row r="666" ht="15.75" customHeight="1">
-      <c r="B666" s="12"/>
+      <c r="B666" s="17"/>
     </row>
     <row r="667" ht="15.75" customHeight="1">
-      <c r="B667" s="12"/>
+      <c r="B667" s="17"/>
     </row>
     <row r="668" ht="15.75" customHeight="1">
-      <c r="B668" s="12"/>
+      <c r="B668" s="17"/>
     </row>
     <row r="669" ht="15.75" customHeight="1">
-      <c r="B669" s="12"/>
+      <c r="B669" s="17"/>
     </row>
     <row r="670" ht="15.75" customHeight="1">
-      <c r="B670" s="12"/>
+      <c r="B670" s="17"/>
     </row>
     <row r="671" ht="15.75" customHeight="1">
-      <c r="B671" s="12"/>
+      <c r="B671" s="17"/>
     </row>
     <row r="672" ht="15.75" customHeight="1">
-      <c r="B672" s="12"/>
+      <c r="B672" s="17"/>
     </row>
     <row r="673" ht="15.75" customHeight="1">
-      <c r="B673" s="12"/>
+      <c r="B673" s="17"/>
     </row>
     <row r="674" ht="15.75" customHeight="1">
-      <c r="B674" s="12"/>
+      <c r="B674" s="17"/>
     </row>
     <row r="675" ht="15.75" customHeight="1">
-      <c r="B675" s="12"/>
+      <c r="B675" s="17"/>
     </row>
     <row r="676" ht="15.75" customHeight="1">
-      <c r="B676" s="12"/>
+      <c r="B676" s="17"/>
     </row>
     <row r="677" ht="15.75" customHeight="1">
-      <c r="B677" s="12"/>
+      <c r="B677" s="17"/>
     </row>
     <row r="678" ht="15.75" customHeight="1">
-      <c r="B678" s="12"/>
+      <c r="B678" s="17"/>
     </row>
     <row r="679" ht="15.75" customHeight="1">
-      <c r="B679" s="12"/>
+      <c r="B679" s="17"/>
     </row>
     <row r="680" ht="15.75" customHeight="1">
-      <c r="B680" s="12"/>
+      <c r="B680" s="17"/>
     </row>
     <row r="681" ht="15.75" customHeight="1">
-      <c r="B681" s="12"/>
+      <c r="B681" s="17"/>
     </row>
     <row r="682" ht="15.75" customHeight="1">
-      <c r="B682" s="12"/>
+      <c r="B682" s="17"/>
     </row>
     <row r="683" ht="15.75" customHeight="1">
-      <c r="B683" s="12"/>
+      <c r="B683" s="17"/>
     </row>
     <row r="684" ht="15.75" customHeight="1">
-      <c r="B684" s="12"/>
+      <c r="B684" s="17"/>
     </row>
     <row r="685" ht="15.75" customHeight="1">
-      <c r="B685" s="12"/>
+      <c r="B685" s="17"/>
     </row>
     <row r="686" ht="15.75" customHeight="1">
-      <c r="B686" s="12"/>
+      <c r="B686" s="17"/>
     </row>
     <row r="687" ht="15.75" customHeight="1">
-      <c r="B687" s="12"/>
+      <c r="B687" s="17"/>
     </row>
     <row r="688" ht="15.75" customHeight="1">
-      <c r="B688" s="12"/>
+      <c r="B688" s="17"/>
     </row>
     <row r="689" ht="15.75" customHeight="1">
-      <c r="B689" s="12"/>
+      <c r="B689" s="17"/>
     </row>
     <row r="690" ht="15.75" customHeight="1">
-      <c r="B690" s="12"/>
+      <c r="B690" s="17"/>
     </row>
     <row r="691" ht="15.75" customHeight="1">
-      <c r="B691" s="12"/>
+      <c r="B691" s="17"/>
     </row>
     <row r="692" ht="15.75" customHeight="1">
-      <c r="B692" s="12"/>
+      <c r="B692" s="17"/>
     </row>
     <row r="693" ht="15.75" customHeight="1">
-      <c r="B693" s="12"/>
+      <c r="B693" s="17"/>
     </row>
     <row r="694" ht="15.75" customHeight="1">
-      <c r="B694" s="12"/>
+      <c r="B694" s="17"/>
     </row>
     <row r="695" ht="15.75" customHeight="1">
-      <c r="B695" s="12"/>
+      <c r="B695" s="17"/>
     </row>
     <row r="696" ht="15.75" customHeight="1">
-      <c r="B696" s="12"/>
+      <c r="B696" s="17"/>
     </row>
     <row r="697" ht="15.75" customHeight="1">
-      <c r="B697" s="12"/>
+      <c r="B697" s="17"/>
     </row>
     <row r="698" ht="15.75" customHeight="1">
-      <c r="B698" s="12"/>
+      <c r="B698" s="17"/>
     </row>
     <row r="699" ht="15.75" customHeight="1">
-      <c r="B699" s="12"/>
+      <c r="B699" s="17"/>
     </row>
     <row r="700" ht="15.75" customHeight="1">
-      <c r="B700" s="12"/>
+      <c r="B700" s="17"/>
     </row>
     <row r="701" ht="15.75" customHeight="1">
-      <c r="B701" s="12"/>
+      <c r="B701" s="17"/>
     </row>
     <row r="702" ht="15.75" customHeight="1">
-      <c r="B702" s="12"/>
+      <c r="B702" s="17"/>
     </row>
     <row r="703" ht="15.75" customHeight="1">
-      <c r="B703" s="12"/>
+      <c r="B703" s="17"/>
     </row>
     <row r="704" ht="15.75" customHeight="1">
-      <c r="B704" s="12"/>
+      <c r="B704" s="17"/>
     </row>
     <row r="705" ht="15.75" customHeight="1">
-      <c r="B705" s="12"/>
+      <c r="B705" s="17"/>
     </row>
     <row r="706" ht="15.75" customHeight="1">
-      <c r="B706" s="12"/>
+      <c r="B706" s="17"/>
     </row>
     <row r="707" ht="15.75" customHeight="1">
-      <c r="B707" s="12"/>
+      <c r="B707" s="17"/>
     </row>
     <row r="708" ht="15.75" customHeight="1">
-      <c r="B708" s="12"/>
+      <c r="B708" s="17"/>
     </row>
     <row r="709" ht="15.75" customHeight="1">
-      <c r="B709" s="12"/>
+      <c r="B709" s="17"/>
     </row>
     <row r="710" ht="15.75" customHeight="1">
-      <c r="B710" s="12"/>
+      <c r="B710" s="17"/>
     </row>
     <row r="711" ht="15.75" customHeight="1">
-      <c r="B711" s="12"/>
+      <c r="B711" s="17"/>
     </row>
     <row r="712" ht="15.75" customHeight="1">
-      <c r="B712" s="12"/>
+      <c r="B712" s="17"/>
     </row>
     <row r="713" ht="15.75" customHeight="1">
-      <c r="B713" s="12"/>
+      <c r="B713" s="17"/>
     </row>
     <row r="714" ht="15.75" customHeight="1">
-      <c r="B714" s="12"/>
+      <c r="B714" s="17"/>
     </row>
     <row r="715" ht="15.75" customHeight="1">
-      <c r="B715" s="12"/>
+      <c r="B715" s="17"/>
     </row>
     <row r="716" ht="15.75" customHeight="1">
-      <c r="B716" s="12"/>
+      <c r="B716" s="17"/>
     </row>
     <row r="717" ht="15.75" customHeight="1">
-      <c r="B717" s="12"/>
+      <c r="B717" s="17"/>
     </row>
     <row r="718" ht="15.75" customHeight="1">
-      <c r="B718" s="12"/>
+      <c r="B718" s="17"/>
     </row>
     <row r="719" ht="15.75" customHeight="1">
-      <c r="B719" s="12"/>
+      <c r="B719" s="17"/>
     </row>
     <row r="720" ht="15.75" customHeight="1">
-      <c r="B720" s="12"/>
+      <c r="B720" s="17"/>
     </row>
     <row r="721" ht="15.75" customHeight="1">
-      <c r="B721" s="12"/>
+      <c r="B721" s="17"/>
     </row>
     <row r="722" ht="15.75" customHeight="1">
-      <c r="B722" s="12"/>
+      <c r="B722" s="17"/>
     </row>
     <row r="723" ht="15.75" customHeight="1">
-      <c r="B723" s="12"/>
+      <c r="B723" s="17"/>
     </row>
     <row r="724" ht="15.75" customHeight="1">
-      <c r="B724" s="12"/>
+      <c r="B724" s="17"/>
     </row>
     <row r="725" ht="15.75" customHeight="1">
-      <c r="B725" s="12"/>
+      <c r="B725" s="17"/>
     </row>
     <row r="726" ht="15.75" customHeight="1">
-      <c r="B726" s="12"/>
+      <c r="B726" s="17"/>
     </row>
     <row r="727" ht="15.75" customHeight="1">
-      <c r="B727" s="12"/>
+      <c r="B727" s="17"/>
     </row>
     <row r="728" ht="15.75" customHeight="1">
-      <c r="B728" s="12"/>
+      <c r="B728" s="17"/>
     </row>
     <row r="729" ht="15.75" customHeight="1">
-      <c r="B729" s="12"/>
+      <c r="B729" s="17"/>
     </row>
     <row r="730" ht="15.75" customHeight="1">
-      <c r="B730" s="12"/>
+      <c r="B730" s="17"/>
     </row>
     <row r="731" ht="15.75" customHeight="1">
-      <c r="B731" s="12"/>
+      <c r="B731" s="17"/>
     </row>
     <row r="732" ht="15.75" customHeight="1">
-      <c r="B732" s="12"/>
+      <c r="B732" s="17"/>
     </row>
     <row r="733" ht="15.75" customHeight="1">
-      <c r="B733" s="12"/>
+      <c r="B733" s="17"/>
     </row>
     <row r="734" ht="15.75" customHeight="1">
-      <c r="B734" s="12"/>
+      <c r="B734" s="17"/>
     </row>
     <row r="735" ht="15.75" customHeight="1">
-      <c r="B735" s="12"/>
+      <c r="B735" s="17"/>
     </row>
     <row r="736" ht="15.75" customHeight="1">
-      <c r="B736" s="12"/>
+      <c r="B736" s="17"/>
     </row>
     <row r="737" ht="15.75" customHeight="1">
-      <c r="B737" s="12"/>
+      <c r="B737" s="17"/>
     </row>
     <row r="738" ht="15.75" customHeight="1">
-      <c r="B738" s="12"/>
+      <c r="B738" s="17"/>
     </row>
     <row r="739" ht="15.75" customHeight="1">
-      <c r="B739" s="12"/>
+      <c r="B739" s="17"/>
     </row>
     <row r="740" ht="15.75" customHeight="1">
-      <c r="B740" s="12"/>
+      <c r="B740" s="17"/>
     </row>
     <row r="741" ht="15.75" customHeight="1">
-      <c r="B741" s="12"/>
+      <c r="B741" s="17"/>
     </row>
     <row r="742" ht="15.75" customHeight="1">
-      <c r="B742" s="12"/>
+      <c r="B742" s="17"/>
     </row>
     <row r="743" ht="15.75" customHeight="1">
-      <c r="B743" s="12"/>
+      <c r="B743" s="17"/>
     </row>
     <row r="744" ht="15.75" customHeight="1">
-      <c r="B744" s="12"/>
+      <c r="B744" s="17"/>
     </row>
     <row r="745" ht="15.75" customHeight="1">
-      <c r="B745" s="12"/>
+      <c r="B745" s="17"/>
     </row>
     <row r="746" ht="15.75" customHeight="1">
-      <c r="B746" s="12"/>
+      <c r="B746" s="17"/>
     </row>
     <row r="747" ht="15.75" customHeight="1">
-      <c r="B747" s="12"/>
+      <c r="B747" s="17"/>
     </row>
     <row r="748" ht="15.75" customHeight="1">
-      <c r="B748" s="12"/>
+      <c r="B748" s="17"/>
     </row>
     <row r="749" ht="15.75" customHeight="1">
-      <c r="B749" s="12"/>
+      <c r="B749" s="17"/>
     </row>
     <row r="750" ht="15.75" customHeight="1">
-      <c r="B750" s="12"/>
+      <c r="B750" s="17"/>
     </row>
     <row r="751" ht="15.75" customHeight="1">
-      <c r="B751" s="12"/>
+      <c r="B751" s="17"/>
     </row>
     <row r="752" ht="15.75" customHeight="1">
-      <c r="B752" s="12"/>
+      <c r="B752" s="17"/>
     </row>
     <row r="753" ht="15.75" customHeight="1">
-      <c r="B753" s="12"/>
+      <c r="B753" s="17"/>
     </row>
     <row r="754" ht="15.75" customHeight="1">
-      <c r="B754" s="12"/>
+      <c r="B754" s="17"/>
     </row>
     <row r="755" ht="15.75" customHeight="1">
-      <c r="B755" s="12"/>
+      <c r="B755" s="17"/>
     </row>
     <row r="756" ht="15.75" customHeight="1">
-      <c r="B756" s="12"/>
+      <c r="B756" s="17"/>
     </row>
     <row r="757" ht="15.75" customHeight="1">
-      <c r="B757" s="12"/>
+      <c r="B757" s="17"/>
     </row>
     <row r="758" ht="15.75" customHeight="1">
-      <c r="B758" s="12"/>
+      <c r="B758" s="17"/>
     </row>
     <row r="759" ht="15.75" customHeight="1">
-      <c r="B759" s="12"/>
+      <c r="B759" s="17"/>
     </row>
     <row r="760" ht="15.75" customHeight="1">
-      <c r="B760" s="12"/>
+      <c r="B760" s="17"/>
     </row>
     <row r="761" ht="15.75" customHeight="1">
-      <c r="B761" s="12"/>
+      <c r="B761" s="17"/>
     </row>
     <row r="762" ht="15.75" customHeight="1">
-      <c r="B762" s="12"/>
+      <c r="B762" s="17"/>
     </row>
     <row r="763" ht="15.75" customHeight="1">
-      <c r="B763" s="12"/>
+      <c r="B763" s="17"/>
     </row>
     <row r="764" ht="15.75" customHeight="1">
-      <c r="B764" s="12"/>
+      <c r="B764" s="17"/>
     </row>
     <row r="765" ht="15.75" customHeight="1">
-      <c r="B765" s="12"/>
+      <c r="B765" s="17"/>
     </row>
     <row r="766" ht="15.75" customHeight="1">
-      <c r="B766" s="12"/>
+      <c r="B766" s="17"/>
     </row>
     <row r="767" ht="15.75" customHeight="1">
-      <c r="B767" s="12"/>
+      <c r="B767" s="17"/>
     </row>
     <row r="768" ht="15.75" customHeight="1">
-      <c r="B768" s="12"/>
+      <c r="B768" s="17"/>
     </row>
     <row r="769" ht="15.75" customHeight="1">
-      <c r="B769" s="12"/>
+      <c r="B769" s="17"/>
     </row>
     <row r="770" ht="15.75" customHeight="1">
-      <c r="B770" s="12"/>
+      <c r="B770" s="17"/>
     </row>
     <row r="771" ht="15.75" customHeight="1">
-      <c r="B771" s="12"/>
+      <c r="B771" s="17"/>
     </row>
     <row r="772" ht="15.75" customHeight="1">
-      <c r="B772" s="12"/>
+      <c r="B772" s="17"/>
     </row>
     <row r="773" ht="15.75" customHeight="1">
-      <c r="B773" s="12"/>
+      <c r="B773" s="17"/>
     </row>
     <row r="774" ht="15.75" customHeight="1">
-      <c r="B774" s="12"/>
+      <c r="B774" s="17"/>
     </row>
     <row r="775" ht="15.75" customHeight="1">
-      <c r="B775" s="12"/>
+      <c r="B775" s="17"/>
     </row>
     <row r="776" ht="15.75" customHeight="1">
-      <c r="B776" s="12"/>
+      <c r="B776" s="17"/>
     </row>
     <row r="777" ht="15.75" customHeight="1">
-      <c r="B777" s="12"/>
+      <c r="B777" s="17"/>
     </row>
     <row r="778" ht="15.75" customHeight="1">
-      <c r="B778" s="12"/>
+      <c r="B778" s="17"/>
     </row>
     <row r="779" ht="15.75" customHeight="1">
-      <c r="B779" s="12"/>
+      <c r="B779" s="17"/>
     </row>
     <row r="780" ht="15.75" customHeight="1">
-      <c r="B780" s="12"/>
+      <c r="B780" s="17"/>
     </row>
     <row r="781" ht="15.75" customHeight="1">
-      <c r="B781" s="12"/>
+      <c r="B781" s="17"/>
     </row>
     <row r="782" ht="15.75" customHeight="1">
-      <c r="B782" s="12"/>
+      <c r="B782" s="17"/>
     </row>
     <row r="783" ht="15.75" customHeight="1">
-      <c r="B783" s="12"/>
+      <c r="B783" s="17"/>
     </row>
     <row r="784" ht="15.75" customHeight="1">
-      <c r="B784" s="12"/>
+      <c r="B784" s="17"/>
     </row>
     <row r="785" ht="15.75" customHeight="1">
-      <c r="B785" s="12"/>
+      <c r="B785" s="17"/>
     </row>
     <row r="786" ht="15.75" customHeight="1">
-      <c r="B786" s="12"/>
+      <c r="B786" s="17"/>
     </row>
     <row r="787" ht="15.75" customHeight="1">
-      <c r="B787" s="12"/>
+      <c r="B787" s="17"/>
     </row>
     <row r="788" ht="15.75" customHeight="1">
-      <c r="B788" s="12"/>
+      <c r="B788" s="17"/>
     </row>
     <row r="789" ht="15.75" customHeight="1">
-      <c r="B789" s="12"/>
+      <c r="B789" s="17"/>
     </row>
     <row r="790" ht="15.75" customHeight="1">
-      <c r="B790" s="12"/>
+      <c r="B790" s="17"/>
     </row>
     <row r="791" ht="15.75" customHeight="1">
-      <c r="B791" s="12"/>
+      <c r="B791" s="17"/>
     </row>
     <row r="792" ht="15.75" customHeight="1">
-      <c r="B792" s="12"/>
+      <c r="B792" s="17"/>
     </row>
     <row r="793" ht="15.75" customHeight="1">
-      <c r="B793" s="12"/>
+      <c r="B793" s="17"/>
     </row>
     <row r="794" ht="15.75" customHeight="1">
-      <c r="B794" s="12"/>
+      <c r="B794" s="17"/>
     </row>
     <row r="795" ht="15.75" customHeight="1">
-      <c r="B795" s="12"/>
+      <c r="B795" s="17"/>
     </row>
     <row r="796" ht="15.75" customHeight="1">
-      <c r="B796" s="12"/>
+      <c r="B796" s="17"/>
     </row>
     <row r="797" ht="15.75" customHeight="1">
-      <c r="B797" s="12"/>
+      <c r="B797" s="17"/>
     </row>
     <row r="798" ht="15.75" customHeight="1">
-      <c r="B798" s="12"/>
+      <c r="B798" s="17"/>
     </row>
     <row r="799" ht="15.75" customHeight="1">
-      <c r="B799" s="12"/>
+      <c r="B799" s="17"/>
     </row>
     <row r="800" ht="15.75" customHeight="1">
-      <c r="B800" s="12"/>
+      <c r="B800" s="17"/>
     </row>
     <row r="801" ht="15.75" customHeight="1">
-      <c r="B801" s="12"/>
+      <c r="B801" s="17"/>
     </row>
     <row r="802" ht="15.75" customHeight="1">
-      <c r="B802" s="12"/>
+      <c r="B802" s="17"/>
     </row>
     <row r="803" ht="15.75" customHeight="1">
-      <c r="B803" s="12"/>
+      <c r="B803" s="17"/>
     </row>
     <row r="804" ht="15.75" customHeight="1">
-      <c r="B804" s="12"/>
+      <c r="B804" s="17"/>
     </row>
     <row r="805" ht="15.75" customHeight="1">
-      <c r="B805" s="12"/>
+      <c r="B805" s="17"/>
     </row>
     <row r="806" ht="15.75" customHeight="1">
-      <c r="B806" s="12"/>
+      <c r="B806" s="17"/>
     </row>
     <row r="807" ht="15.75" customHeight="1">
-      <c r="B807" s="12"/>
+      <c r="B807" s="17"/>
     </row>
     <row r="808" ht="15.75" customHeight="1">
-      <c r="B808" s="12"/>
+      <c r="B808" s="17"/>
     </row>
     <row r="809" ht="15.75" customHeight="1">
-      <c r="B809" s="12"/>
+      <c r="B809" s="17"/>
     </row>
     <row r="810" ht="15.75" customHeight="1">
-      <c r="B810" s="12"/>
+      <c r="B810" s="17"/>
     </row>
     <row r="811" ht="15.75" customHeight="1">
-      <c r="B811" s="12"/>
+      <c r="B811" s="17"/>
     </row>
     <row r="812" ht="15.75" customHeight="1">
-      <c r="B812" s="12"/>
+      <c r="B812" s="17"/>
     </row>
     <row r="813" ht="15.75" customHeight="1">
-      <c r="B813" s="12"/>
+      <c r="B813" s="17"/>
     </row>
     <row r="814" ht="15.75" customHeight="1">
-      <c r="B814" s="12"/>
+      <c r="B814" s="17"/>
     </row>
     <row r="815" ht="15.75" customHeight="1">
-      <c r="B815" s="12"/>
+      <c r="B815" s="17"/>
     </row>
     <row r="816" ht="15.75" customHeight="1">
-      <c r="B816" s="12"/>
+      <c r="B816" s="17"/>
     </row>
     <row r="817" ht="15.75" customHeight="1">
-      <c r="B817" s="12"/>
+      <c r="B817" s="17"/>
     </row>
     <row r="818" ht="15.75" customHeight="1">
-      <c r="B818" s="12"/>
+      <c r="B818" s="17"/>
     </row>
     <row r="819" ht="15.75" customHeight="1">
-      <c r="B819" s="12"/>
+      <c r="B819" s="17"/>
     </row>
     <row r="820" ht="15.75" customHeight="1">
-      <c r="B820" s="12"/>
+      <c r="B820" s="17"/>
     </row>
     <row r="821" ht="15.75" customHeight="1">
-      <c r="B821" s="12"/>
+      <c r="B821" s="17"/>
     </row>
     <row r="822" ht="15.75" customHeight="1">
-      <c r="B822" s="12"/>
+      <c r="B822" s="17"/>
     </row>
     <row r="823" ht="15.75" customHeight="1">
-      <c r="B823" s="12"/>
+      <c r="B823" s="17"/>
     </row>
     <row r="824" ht="15.75" customHeight="1">
-      <c r="B824" s="12"/>
+      <c r="B824" s="17"/>
     </row>
     <row r="825" ht="15.75" customHeight="1">
-      <c r="B825" s="12"/>
+      <c r="B825" s="17"/>
     </row>
     <row r="826" ht="15.75" customHeight="1">
-      <c r="B826" s="12"/>
+      <c r="B826" s="17"/>
     </row>
     <row r="827" ht="15.75" customHeight="1">
-      <c r="B827" s="12"/>
+      <c r="B827" s="17"/>
     </row>
     <row r="828" ht="15.75" customHeight="1">
-      <c r="B828" s="12"/>
+      <c r="B828" s="17"/>
     </row>
     <row r="829" ht="15.75" customHeight="1">
-      <c r="B829" s="12"/>
+      <c r="B829" s="17"/>
     </row>
     <row r="830" ht="15.75" customHeight="1">
-      <c r="B830" s="12"/>
+      <c r="B830" s="17"/>
     </row>
     <row r="831" ht="15.75" customHeight="1">
-      <c r="B831" s="12"/>
+      <c r="B831" s="17"/>
     </row>
     <row r="832" ht="15.75" customHeight="1">
-      <c r="B832" s="12"/>
+      <c r="B832" s="17"/>
     </row>
     <row r="833" ht="15.75" customHeight="1">
-      <c r="B833" s="12"/>
+      <c r="B833" s="17"/>
     </row>
     <row r="834" ht="15.75" customHeight="1">
-      <c r="B834" s="12"/>
+      <c r="B834" s="17"/>
     </row>
     <row r="835" ht="15.75" customHeight="1">
-      <c r="B835" s="12"/>
+      <c r="B835" s="17"/>
     </row>
     <row r="836" ht="15.75" customHeight="1">
-      <c r="B836" s="12"/>
+      <c r="B836" s="17"/>
     </row>
     <row r="837" ht="15.75" customHeight="1">
-      <c r="B837" s="12"/>
+      <c r="B837" s="17"/>
     </row>
     <row r="838" ht="15.75" customHeight="1">
-      <c r="B838" s="12"/>
+      <c r="B838" s="17"/>
     </row>
     <row r="839" ht="15.75" customHeight="1">
-      <c r="B839" s="12"/>
+      <c r="B839" s="17"/>
     </row>
     <row r="840" ht="15.75" customHeight="1">
-      <c r="B840" s="12"/>
+      <c r="B840" s="17"/>
     </row>
     <row r="841" ht="15.75" customHeight="1">
-      <c r="B841" s="12"/>
+      <c r="B841" s="17"/>
     </row>
     <row r="842" ht="15.75" customHeight="1">
-      <c r="B842" s="12"/>
+      <c r="B842" s="17"/>
     </row>
     <row r="843" ht="15.75" customHeight="1">
-      <c r="B843" s="12"/>
+      <c r="B843" s="17"/>
     </row>
     <row r="844" ht="15.75" customHeight="1">
-      <c r="B844" s="12"/>
+      <c r="B844" s="17"/>
     </row>
     <row r="845" ht="15.75" customHeight="1">
-      <c r="B845" s="12"/>
+      <c r="B845" s="17"/>
     </row>
     <row r="846" ht="15.75" customHeight="1">
-      <c r="B846" s="12"/>
+      <c r="B846" s="17"/>
     </row>
     <row r="847" ht="15.75" customHeight="1">
-      <c r="B847" s="12"/>
+      <c r="B847" s="17"/>
     </row>
     <row r="848" ht="15.75" customHeight="1">
-      <c r="B848" s="12"/>
+      <c r="B848" s="17"/>
     </row>
     <row r="849" ht="15.75" customHeight="1">
-      <c r="B849" s="12"/>
+      <c r="B849" s="17"/>
     </row>
     <row r="850" ht="15.75" customHeight="1">
-      <c r="B850" s="12"/>
+      <c r="B850" s="17"/>
     </row>
     <row r="851" ht="15.75" customHeight="1">
-      <c r="B851" s="12"/>
+      <c r="B851" s="17"/>
     </row>
     <row r="852" ht="15.75" customHeight="1">
-      <c r="B852" s="12"/>
+      <c r="B852" s="17"/>
     </row>
     <row r="853" ht="15.75" customHeight="1">
-      <c r="B853" s="12"/>
+      <c r="B853" s="17"/>
     </row>
     <row r="854" ht="15.75" customHeight="1">
-      <c r="B854" s="12"/>
+      <c r="B854" s="17"/>
     </row>
     <row r="855" ht="15.75" customHeight="1">
-      <c r="B855" s="12"/>
+      <c r="B855" s="17"/>
     </row>
     <row r="856" ht="15.75" customHeight="1">
-      <c r="B856" s="12"/>
+      <c r="B856" s="17"/>
     </row>
     <row r="857" ht="15.75" customHeight="1">
-      <c r="B857" s="12"/>
+      <c r="B857" s="17"/>
     </row>
     <row r="858" ht="15.75" customHeight="1">
-      <c r="B858" s="12"/>
+      <c r="B858" s="17"/>
     </row>
     <row r="859" ht="15.75" customHeight="1">
-      <c r="B859" s="12"/>
+      <c r="B859" s="17"/>
     </row>
     <row r="860" ht="15.75" customHeight="1">
-      <c r="B860" s="12"/>
+      <c r="B860" s="17"/>
     </row>
     <row r="861" ht="15.75" customHeight="1">
-      <c r="B861" s="12"/>
+      <c r="B861" s="17"/>
     </row>
     <row r="862" ht="15.75" customHeight="1">
-      <c r="B862" s="12"/>
+      <c r="B862" s="17"/>
     </row>
     <row r="863" ht="15.75" customHeight="1">
-      <c r="B863" s="12"/>
+      <c r="B863" s="17"/>
     </row>
     <row r="864" ht="15.75" customHeight="1">
-      <c r="B864" s="12"/>
+      <c r="B864" s="17"/>
     </row>
     <row r="865" ht="15.75" customHeight="1">
-      <c r="B865" s="12"/>
+      <c r="B865" s="17"/>
     </row>
     <row r="866" ht="15.75" customHeight="1">
-      <c r="B866" s="12"/>
+      <c r="B866" s="17"/>
     </row>
     <row r="867" ht="15.75" customHeight="1">
-      <c r="B867" s="12"/>
+      <c r="B867" s="17"/>
     </row>
     <row r="868" ht="15.75" customHeight="1">
-      <c r="B868" s="12"/>
+      <c r="B868" s="17"/>
     </row>
     <row r="869" ht="15.75" customHeight="1">
-      <c r="B869" s="12"/>
+      <c r="B869" s="17"/>
     </row>
     <row r="870" ht="15.75" customHeight="1">
-      <c r="B870" s="12"/>
+      <c r="B870" s="17"/>
     </row>
     <row r="871" ht="15.75" customHeight="1">
-      <c r="B871" s="12"/>
+      <c r="B871" s="17"/>
     </row>
     <row r="872" ht="15.75" customHeight="1">
-      <c r="B872" s="12"/>
+      <c r="B872" s="17"/>
     </row>
     <row r="873" ht="15.75" customHeight="1">
-      <c r="B873" s="12"/>
+      <c r="B873" s="17"/>
     </row>
     <row r="874" ht="15.75" customHeight="1">
-      <c r="B874" s="12"/>
+      <c r="B874" s="17"/>
     </row>
     <row r="875" ht="15.75" customHeight="1">
-      <c r="B875" s="12"/>
+      <c r="B875" s="17"/>
     </row>
     <row r="876" ht="15.75" customHeight="1">
-      <c r="B876" s="12"/>
+      <c r="B876" s="17"/>
     </row>
     <row r="877" ht="15.75" customHeight="1">
-      <c r="B877" s="12"/>
+      <c r="B877" s="17"/>
     </row>
     <row r="878" ht="15.75" customHeight="1">
-      <c r="B878" s="12"/>
+      <c r="B878" s="17"/>
     </row>
     <row r="879" ht="15.75" customHeight="1">
-      <c r="B879" s="12"/>
+      <c r="B879" s="17"/>
     </row>
     <row r="880" ht="15.75" customHeight="1">
-      <c r="B880" s="12"/>
+      <c r="B880" s="17"/>
     </row>
     <row r="881" ht="15.75" customHeight="1">
-      <c r="B881" s="12"/>
+      <c r="B881" s="17"/>
     </row>
     <row r="882" ht="15.75" customHeight="1">
-      <c r="B882" s="12"/>
+      <c r="B882" s="17"/>
     </row>
     <row r="883" ht="15.75" customHeight="1">
-      <c r="B883" s="12"/>
+      <c r="B883" s="17"/>
     </row>
     <row r="884" ht="15.75" customHeight="1">
-      <c r="B884" s="12"/>
+      <c r="B884" s="17"/>
     </row>
     <row r="885" ht="15.75" customHeight="1">
-      <c r="B885" s="12"/>
+      <c r="B885" s="17"/>
     </row>
     <row r="886" ht="15.75" customHeight="1">
-      <c r="B886" s="12"/>
+      <c r="B886" s="17"/>
     </row>
     <row r="887" ht="15.75" customHeight="1">
-      <c r="B887" s="12"/>
+      <c r="B887" s="17"/>
     </row>
     <row r="888" ht="15.75" customHeight="1">
-      <c r="B888" s="12"/>
+      <c r="B888" s="17"/>
     </row>
     <row r="889" ht="15.75" customHeight="1">
-      <c r="B889" s="12"/>
+      <c r="B889" s="17"/>
     </row>
     <row r="890" ht="15.75" customHeight="1">
-      <c r="B890" s="12"/>
+      <c r="B890" s="17"/>
     </row>
     <row r="891" ht="15.75" customHeight="1">
-      <c r="B891" s="12"/>
+      <c r="B891" s="17"/>
     </row>
     <row r="892" ht="15.75" customHeight="1">
-      <c r="B892" s="12"/>
+      <c r="B892" s="17"/>
     </row>
     <row r="893" ht="15.75" customHeight="1">
-      <c r="B893" s="12"/>
+      <c r="B893" s="17"/>
     </row>
     <row r="894" ht="15.75" customHeight="1">
-      <c r="B894" s="12"/>
+      <c r="B894" s="17"/>
     </row>
     <row r="895" ht="15.75" customHeight="1">
-      <c r="B895" s="12"/>
+      <c r="B895" s="17"/>
     </row>
     <row r="896" ht="15.75" customHeight="1">
-      <c r="B896" s="12"/>
+      <c r="B896" s="17"/>
     </row>
     <row r="897" ht="15.75" customHeight="1">
-      <c r="B897" s="12"/>
+      <c r="B897" s="17"/>
     </row>
     <row r="898" ht="15.75" customHeight="1">
-      <c r="B898" s="12"/>
+      <c r="B898" s="17"/>
     </row>
     <row r="899" ht="15.75" customHeight="1">
-      <c r="B899" s="12"/>
+      <c r="B899" s="17"/>
     </row>
     <row r="900" ht="15.75" customHeight="1">
-      <c r="B900" s="12"/>
+      <c r="B900" s="17"/>
     </row>
     <row r="901" ht="15.75" customHeight="1">
-      <c r="B901" s="12"/>
+      <c r="B901" s="17"/>
     </row>
     <row r="902" ht="15.75" customHeight="1">
-      <c r="B902" s="12"/>
+      <c r="B902" s="17"/>
     </row>
     <row r="903" ht="15.75" customHeight="1">
-      <c r="B903" s="12"/>
+      <c r="B903" s="17"/>
     </row>
     <row r="904" ht="15.75" customHeight="1">
-      <c r="B904" s="12"/>
+      <c r="B904" s="17"/>
     </row>
     <row r="905" ht="15.75" customHeight="1">
-      <c r="B905" s="12"/>
+      <c r="B905" s="17"/>
     </row>
     <row r="906" ht="15.75" customHeight="1">
-      <c r="B906" s="12"/>
+      <c r="B906" s="17"/>
     </row>
     <row r="907" ht="15.75" customHeight="1">
-      <c r="B907" s="12"/>
+      <c r="B907" s="17"/>
     </row>
     <row r="908" ht="15.75" customHeight="1">
-      <c r="B908" s="12"/>
+      <c r="B908" s="17"/>
     </row>
     <row r="909" ht="15.75" customHeight="1">
-      <c r="B909" s="12"/>
+      <c r="B909" s="17"/>
     </row>
     <row r="910" ht="15.75" customHeight="1">
-      <c r="B910" s="12"/>
+      <c r="B910" s="17"/>
     </row>
     <row r="911" ht="15.75" customHeight="1">
-      <c r="B911" s="12"/>
+      <c r="B911" s="17"/>
     </row>
     <row r="912" ht="15.75" customHeight="1">
-      <c r="B912" s="12"/>
+      <c r="B912" s="17"/>
     </row>
     <row r="913" ht="15.75" customHeight="1">
-      <c r="B913" s="12"/>
+      <c r="B913" s="17"/>
     </row>
     <row r="914" ht="15.75" customHeight="1">
-      <c r="B914" s="12"/>
+      <c r="B914" s="17"/>
     </row>
     <row r="915" ht="15.75" customHeight="1">
-      <c r="B915" s="12"/>
+      <c r="B915" s="17"/>
     </row>
     <row r="916" ht="15.75" customHeight="1">
-      <c r="B916" s="12"/>
+      <c r="B916" s="17"/>
     </row>
     <row r="917" ht="15.75" customHeight="1">
-      <c r="B917" s="12"/>
+      <c r="B917" s="17"/>
     </row>
     <row r="918" ht="15.75" customHeight="1">
-      <c r="B918" s="12"/>
+      <c r="B918" s="17"/>
     </row>
     <row r="919" ht="15.75" customHeight="1">
-      <c r="B919" s="12"/>
+      <c r="B919" s="17"/>
     </row>
     <row r="920" ht="15.75" customHeight="1">
-      <c r="B920" s="12"/>
+      <c r="B920" s="17"/>
     </row>
     <row r="921" ht="15.75" customHeight="1">
-      <c r="B921" s="12"/>
+      <c r="B921" s="17"/>
     </row>
     <row r="922" ht="15.75" customHeight="1">
-      <c r="B922" s="12"/>
+      <c r="B922" s="17"/>
     </row>
     <row r="923" ht="15.75" customHeight="1">
-      <c r="B923" s="12"/>
+      <c r="B923" s="17"/>
     </row>
     <row r="924" ht="15.75" customHeight="1">
-      <c r="B924" s="12"/>
+      <c r="B924" s="17"/>
     </row>
     <row r="925" ht="15.75" customHeight="1">
-      <c r="B925" s="12"/>
+      <c r="B925" s="17"/>
     </row>
     <row r="926" ht="15.75" customHeight="1">
-      <c r="B926" s="12"/>
+      <c r="B926" s="17"/>
     </row>
     <row r="927" ht="15.75" customHeight="1">
-      <c r="B927" s="12"/>
+      <c r="B927" s="17"/>
     </row>
     <row r="928" ht="15.75" customHeight="1">
-      <c r="B928" s="12"/>
+      <c r="B928" s="17"/>
     </row>
     <row r="929" ht="15.75" customHeight="1">
-      <c r="B929" s="12"/>
+      <c r="B929" s="17"/>
     </row>
     <row r="930" ht="15.75" customHeight="1">
-      <c r="B930" s="12"/>
+      <c r="B930" s="17"/>
     </row>
     <row r="931" ht="15.75" customHeight="1">
-      <c r="B931" s="12"/>
+      <c r="B931" s="17"/>
     </row>
     <row r="932" ht="15.75" customHeight="1">
-      <c r="B932" s="12"/>
+      <c r="B932" s="17"/>
     </row>
     <row r="933" ht="15.75" customHeight="1">
-      <c r="B933" s="12"/>
+      <c r="B933" s="17"/>
     </row>
     <row r="934" ht="15.75" customHeight="1">
-      <c r="B934" s="12"/>
+      <c r="B934" s="17"/>
     </row>
     <row r="935" ht="15.75" customHeight="1">
-      <c r="B935" s="12"/>
+      <c r="B935" s="17"/>
     </row>
     <row r="936" ht="15.75" customHeight="1">
-      <c r="B936" s="12"/>
+      <c r="B936" s="17"/>
     </row>
     <row r="937" ht="15.75" customHeight="1">
-      <c r="B937" s="12"/>
+      <c r="B937" s="17"/>
     </row>
     <row r="938" ht="15.75" customHeight="1">
-      <c r="B938" s="12"/>
+      <c r="B938" s="17"/>
     </row>
     <row r="939" ht="15.75" customHeight="1">
-      <c r="B939" s="12"/>
+      <c r="B939" s="17"/>
     </row>
     <row r="940" ht="15.75" customHeight="1">
-      <c r="B940" s="12"/>
+      <c r="B940" s="17"/>
     </row>
     <row r="941" ht="15.75" customHeight="1">
-      <c r="B941" s="12"/>
+      <c r="B941" s="17"/>
     </row>
     <row r="942" ht="15.75" customHeight="1">
-      <c r="B942" s="12"/>
+      <c r="B942" s="17"/>
     </row>
     <row r="943" ht="15.75" customHeight="1">
-      <c r="B943" s="12"/>
+      <c r="B943" s="17"/>
     </row>
     <row r="944" ht="15.75" customHeight="1">
-      <c r="B944" s="12"/>
+      <c r="B944" s="17"/>
     </row>
     <row r="945" ht="15.75" customHeight="1">
-      <c r="B945" s="12"/>
+      <c r="B945" s="17"/>
     </row>
     <row r="946" ht="15.75" customHeight="1">
-      <c r="B946" s="12"/>
+      <c r="B946" s="17"/>
     </row>
     <row r="947" ht="15.75" customHeight="1">
-      <c r="B947" s="12"/>
+      <c r="B947" s="17"/>
     </row>
     <row r="948" ht="15.75" customHeight="1">
-      <c r="B948" s="12"/>
+      <c r="B948" s="17"/>
     </row>
     <row r="949" ht="15.75" customHeight="1">
-      <c r="B949" s="12"/>
+      <c r="B949" s="17"/>
     </row>
     <row r="950" ht="15.75" customHeight="1">
-      <c r="B950" s="12"/>
+      <c r="B950" s="17"/>
     </row>
     <row r="951" ht="15.75" customHeight="1">
-      <c r="B951" s="12"/>
+      <c r="B951" s="17"/>
     </row>
     <row r="952" ht="15.75" customHeight="1">
-      <c r="B952" s="12"/>
+      <c r="B952" s="17"/>
     </row>
     <row r="953" ht="15.75" customHeight="1">
-      <c r="B953" s="12"/>
+      <c r="B953" s="17"/>
     </row>
     <row r="954" ht="15.75" customHeight="1">
-      <c r="B954" s="12"/>
+      <c r="B954" s="17"/>
     </row>
     <row r="955" ht="15.75" customHeight="1">
-      <c r="B955" s="12"/>
+      <c r="B955" s="17"/>
     </row>
     <row r="956" ht="15.75" customHeight="1">
-      <c r="B956" s="12"/>
+      <c r="B956" s="17"/>
     </row>
     <row r="957" ht="15.75" customHeight="1">
-      <c r="B957" s="12"/>
+      <c r="B957" s="17"/>
     </row>
     <row r="958" ht="15.75" customHeight="1">
-      <c r="B958" s="12"/>
+      <c r="B958" s="17"/>
     </row>
     <row r="959" ht="15.75" customHeight="1">
-      <c r="B959" s="12"/>
+      <c r="B959" s="17"/>
     </row>
     <row r="960" ht="15.75" customHeight="1">
-      <c r="B960" s="12"/>
+      <c r="B960" s="17"/>
     </row>
     <row r="961" ht="15.75" customHeight="1">
-      <c r="B961" s="12"/>
+      <c r="B961" s="17"/>
     </row>
     <row r="962" ht="15.75" customHeight="1">
-      <c r="B962" s="12"/>
+      <c r="B962" s="17"/>
     </row>
     <row r="963" ht="15.75" customHeight="1">
-      <c r="B963" s="12"/>
+      <c r="B963" s="17"/>
     </row>
     <row r="964" ht="15.75" customHeight="1">
-      <c r="B964" s="12"/>
+      <c r="B964" s="17"/>
     </row>
     <row r="965" ht="15.75" customHeight="1">
-      <c r="B965" s="12"/>
+      <c r="B965" s="17"/>
     </row>
     <row r="966" ht="15.75" customHeight="1">
-      <c r="B966" s="12"/>
+      <c r="B966" s="17"/>
     </row>
     <row r="967" ht="15.75" customHeight="1">
-      <c r="B967" s="12"/>
+      <c r="B967" s="17"/>
     </row>
     <row r="968" ht="15.75" customHeight="1">
-      <c r="B968" s="12"/>
+      <c r="B968" s="17"/>
     </row>
     <row r="969" ht="15.75" customHeight="1">
-      <c r="B969" s="12"/>
+      <c r="B969" s="17"/>
     </row>
     <row r="970" ht="15.75" customHeight="1">
-      <c r="B970" s="12"/>
+      <c r="B970" s="17"/>
     </row>
     <row r="971" ht="15.75" customHeight="1">
-      <c r="B971" s="12"/>
+      <c r="B971" s="17"/>
     </row>
     <row r="972" ht="15.75" customHeight="1">
-      <c r="B972" s="12"/>
+      <c r="B972" s="17"/>
     </row>
     <row r="973" ht="15.75" customHeight="1">
-      <c r="B973" s="12"/>
+      <c r="B973" s="17"/>
     </row>
     <row r="974" ht="15.75" customHeight="1">
-      <c r="B974" s="12"/>
+      <c r="B974" s="17"/>
     </row>
     <row r="975" ht="15.75" customHeight="1">
-      <c r="B975" s="12"/>
+      <c r="B975" s="17"/>
     </row>
     <row r="976" ht="15.75" customHeight="1">
-      <c r="B976" s="12"/>
+      <c r="B976" s="17"/>
     </row>
     <row r="977" ht="15.75" customHeight="1">
-      <c r="B977" s="12"/>
+      <c r="B977" s="17"/>
     </row>
     <row r="978" ht="15.75" customHeight="1">
-      <c r="B978" s="12"/>
+      <c r="B978" s="17"/>
     </row>
     <row r="979" ht="15.75" customHeight="1">
-      <c r="B979" s="12"/>
+      <c r="B979" s="17"/>
     </row>
     <row r="980" ht="15.75" customHeight="1">
-      <c r="B980" s="12"/>
+      <c r="B980" s="17"/>
     </row>
     <row r="981" ht="15.75" customHeight="1">
-      <c r="B981" s="12"/>
+      <c r="B981" s="17"/>
     </row>
     <row r="982" ht="15.75" customHeight="1">
-      <c r="B982" s="12"/>
+      <c r="B982" s="17"/>
     </row>
     <row r="983" ht="15.75" customHeight="1">
-      <c r="B983" s="12"/>
+      <c r="B983" s="17"/>
     </row>
     <row r="984" ht="15.75" customHeight="1">
-      <c r="B984" s="12"/>
+      <c r="B984" s="17"/>
     </row>
     <row r="985" ht="15.75" customHeight="1">
-      <c r="B985" s="12"/>
+      <c r="B985" s="17"/>
     </row>
     <row r="986" ht="15.75" customHeight="1">
-      <c r="B986" s="12"/>
+      <c r="B986" s="17"/>
     </row>
     <row r="987" ht="15.75" customHeight="1">
-      <c r="B987" s="12"/>
+      <c r="B987" s="17"/>
     </row>
     <row r="988" ht="15.75" customHeight="1">
-      <c r="B988" s="12"/>
+      <c r="B988" s="17"/>
     </row>
     <row r="989" ht="15.75" customHeight="1">
-      <c r="B989" s="12"/>
+      <c r="B989" s="17"/>
     </row>
     <row r="990" ht="15.75" customHeight="1">
-      <c r="B990" s="12"/>
+      <c r="B990" s="17"/>
     </row>
     <row r="991" ht="15.75" customHeight="1">
-      <c r="B991" s="12"/>
+      <c r="B991" s="17"/>
     </row>
     <row r="992" ht="15.75" customHeight="1">
-      <c r="B992" s="12"/>
+      <c r="B992" s="17"/>
     </row>
     <row r="993" ht="15.75" customHeight="1">
-      <c r="B993" s="12"/>
+      <c r="B993" s="17"/>
     </row>
     <row r="994" ht="15.75" customHeight="1">
-      <c r="B994" s="12"/>
+      <c r="B994" s="17"/>
     </row>
     <row r="995" ht="15.75" customHeight="1">
-      <c r="B995" s="12"/>
+      <c r="B995" s="17"/>
     </row>
     <row r="996" ht="15.75" customHeight="1">
-      <c r="B996" s="12"/>
+      <c r="B996" s="17"/>
     </row>
     <row r="997" ht="15.75" customHeight="1">
-      <c r="B997" s="12"/>
+      <c r="B997" s="17"/>
     </row>
     <row r="998" ht="15.75" customHeight="1">
-      <c r="B998" s="12"/>
+      <c r="B998" s="17"/>
     </row>
     <row r="999" ht="15.75" customHeight="1">
-      <c r="B999" s="12"/>
+      <c r="B999" s="17"/>
     </row>
     <row r="1000" ht="15.75" customHeight="1">
-      <c r="B1000" s="12"/>
+      <c r="B1000" s="17"/>
     </row>
     <row r="1001" ht="15.75" customHeight="1">
-      <c r="B1001" s="12"/>
+      <c r="B1001" s="17"/>
     </row>
     <row r="1002" ht="15.75" customHeight="1">
-      <c r="B1002" s="12"/>
+      <c r="B1002" s="17"/>
+    </row>
+    <row r="1003" ht="15.75" customHeight="1">
+      <c r="B1003" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -9263,8 +9452,8 @@
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A23:E23"/>
     <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A28:E28"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>